<commit_message>
Deleted first RVM requirement
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Description</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Demo</t>
-  </si>
-  <si>
-    <t>CONOPS Step (If Applicable)</t>
   </si>
   <si>
     <t>Examine</t>
@@ -130,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -210,17 +207,6 @@
       <top style="thin">
         <color theme="0"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -315,10 +301,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,41 +314,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -780,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -792,56 +778,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="B3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="B4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>23</v>
       </c>
       <c r="B5" s="21">
         <v>41582</v>
@@ -853,24 +839,24 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1017,474 +1003,432 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
+      <c r="B20" s="20"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+      <c r="B29" s="20"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="7"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="7"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="20"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="20"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="7"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="7"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="7"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="B36" s="20"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="7"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="7"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
+      <c r="B38" s="20"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="7"/>
+      <c r="H38" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="D1:G1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1496,25 +1440,25 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
@@ -1523,14 +1467,14 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="10"/>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1541,12 +1485,14 @@
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>

</xml_diff>

<commit_message>
Added propulsion requirements in Stage 1
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="113">
   <si>
     <t>Verification Method</t>
   </si>
@@ -403,6 +403,77 @@
   </si>
   <si>
     <t>RCL-TST-RVM5</t>
+  </si>
+  <si>
+    <t>The deployer shall not be used to secure any CubeSat deployables</t>
+  </si>
+  <si>
+    <t>Propulsion</t>
+  </si>
+  <si>
+    <t>RCL-PRP-RVM1</t>
+  </si>
+  <si>
+    <t>RCL-PRP-RVM2</t>
+  </si>
+  <si>
+    <t>Static Thrust testing will be performed with the flight pressure vessal at a pressure of at least 1x10^-4 Torr prior to CubeSat integration</t>
+  </si>
+  <si>
+    <t>Propulsin</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thermal cycle testing will be performed with the pressure vessal between temperautres of -30 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>⁰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">C and 70 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>⁰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>C for a total of two cycles or 10 hours</t>
+    </r>
+  </si>
+  <si>
+    <t>RCL-PRP-RVM3</t>
+  </si>
+  <si>
+    <t>On Orbit Requirements</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>Ground Station</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1343,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,12 +1444,20 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
@@ -1515,7 +1594,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,55 +2601,55 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -2578,7 +2657,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>32</v>
@@ -2594,25 +2673,25 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="59.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5" t="s">
         <v>75</v>
@@ -2626,7 +2705,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>32</v>
@@ -2642,15 +2721,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>92</v>
+      <c r="C15" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>32</v>
@@ -2671,13 +2750,13 @@
         <v>30</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
@@ -2687,45 +2766,45 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>78</v>
+        <v>108</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>24</v>
@@ -2735,205 +2814,229 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="24" t="s">
-        <v>80</v>
+        <v>59</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="B23" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C23" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D23" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="5" t="s">
+      <c r="E23" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B24" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C24" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D24" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="5" t="s">
+      <c r="E24" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B25" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C25" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D25" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="5" t="s">
+      <c r="E25" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+    <row r="26" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B26" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C26" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D26" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="30" t="s">
+      <c r="E26" s="30"/>
+      <c r="F26" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+    <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5" t="s">
-        <v>39</v>
+      <c r="B28" s="27"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2949,7 +3052,7 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2965,7 +3068,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2981,7 +3084,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2997,7 +3100,7 @@
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3013,7 +3116,7 @@
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3029,7 +3132,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3045,7 +3148,7 @@
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3061,7 +3164,7 @@
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3077,7 +3180,7 @@
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -3093,7 +3196,7 @@
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3109,7 +3212,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3125,7 +3228,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
       <c r="J40" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3141,7 +3244,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3157,7 +3260,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3173,6 +3276,54 @@
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3181,7 +3332,7 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A27:J27"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>

</xml_diff>

<commit_message>
Justified slew rate of 1 deg/sec, as noted in NAV folder reference material
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -324,9 +324,6 @@
     <t>RCL-PRP-RVM1</t>
   </si>
   <si>
-    <t>Static Thrust testing will be performed with the flight pressure vessel at a pressure no greater than 1x10^-4 Torr prior to CubeSat integration</t>
-  </si>
-  <si>
     <t>RCL-PRP-RVM2</t>
   </si>
   <si>
@@ -473,12 +470,6 @@
   </si>
   <si>
     <t>RCL-SS-RVM1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual CubeSat system shall be able to stabilize roll rate about each of the primary axes to less than 1 deg/s </t>
-  </si>
-  <si>
-    <t>Need Rationale</t>
   </si>
   <si>
     <t>RCL-SS-RVM2</t>
@@ -621,12 +612,21 @@
       <t>C for a total of two cycles or 10 hours</t>
     </r>
   </si>
+  <si>
+    <t>Static Thrust testing will be performed with the flight pressure vessel  prior to CubeSat integration at a pressure no greater than 1x10^-4 Torr</t>
+  </si>
+  <si>
+    <t>Reference Material (NAV Folder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual CubeSat system shall achieve a local slew rate of less than 1 deg/s </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -670,6 +670,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -691,7 +696,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -762,21 +767,6 @@
         <color indexed="8"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="double">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -896,7 +886,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -951,35 +941,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -988,32 +968,45 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1670,67 +1663,67 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="30">
         <v>41582</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="35"/>
+      <c r="B8" s="31"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
@@ -1947,12 +1940,12 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="6">
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="A8:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1965,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IS314"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1984,36 +1977,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:253">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="40" t="s">
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="35" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:253">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="8" t="s">
         <v>55</v>
       </c>
@@ -2026,44 +2019,44 @@
       <c r="H2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="37"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:253">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:253" s="10" customFormat="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30" t="s">
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30" t="s">
+      <c r="I4" s="26"/>
+      <c r="J4" s="26" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2074,8 +2067,8 @@
       <c r="B5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>152</v>
+      <c r="C5" s="27" t="s">
+        <v>149</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>64</v>
@@ -2086,8 +2079,8 @@
       <c r="H5" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="30" t="s">
+      <c r="I5" s="24"/>
+      <c r="J5" s="26" t="s">
         <v>69</v>
       </c>
       <c r="M5" s="14"/>
@@ -2159,8 +2152,8 @@
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="30" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="26" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2183,57 +2176,57 @@
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="30" t="s">
+      <c r="I7" s="23"/>
+      <c r="J7" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:253">
       <c r="A8" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>89</v>
+        <v>39</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11" t="s">
+      <c r="F8" s="11" t="s">
         <v>62</v>
       </c>
+      <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
-      <c r="J8" s="30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:253">
+      <c r="J8" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:253" ht="30">
       <c r="A9" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>64</v>
+        <v>99</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>100</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="G9" s="11"/>
-      <c r="H9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I9" s="27"/>
-      <c r="J9" s="30" t="s">
-        <v>65</v>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:253">
@@ -2243,32 +2236,32 @@
       <c r="B10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>154</v>
+      <c r="C10" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I10" s="27"/>
-      <c r="J10" s="30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:253" ht="30">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:253">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>72</v>
+      <c r="C11" s="12" t="s">
+        <v>150</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>64</v>
@@ -2279,20 +2272,20 @@
       <c r="H11" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:253" ht="30">
+      <c r="I11" s="23"/>
+      <c r="J11" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:253">
       <c r="A12" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>70</v>
+      <c r="C12" s="12" t="s">
+        <v>151</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>64</v>
@@ -2303,12 +2296,12 @@
       <c r="H12" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="27"/>
-      <c r="J12" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:253">
+      <c r="I12" s="23"/>
+      <c r="J12" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:253" ht="30">
       <c r="A13" s="11" t="s">
         <v>12</v>
       </c>
@@ -2316,117 +2309,117 @@
         <v>41</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="30" t="s">
-        <v>79</v>
+      <c r="I13" s="23"/>
+      <c r="J13" s="26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:253" ht="30">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="16" t="s">
+      <c r="C14" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="V14" s="29"/>
-    </row>
-    <row r="15" spans="1:253" ht="30">
+      <c r="I14" s="23"/>
+      <c r="J14" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="V14" s="25"/>
+    </row>
+    <row r="15" spans="1:253">
       <c r="A15" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="11"/>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="11"/>
+      <c r="G15" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="11"/>
       <c r="H15" s="11"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="30" t="s">
-        <v>83</v>
+      <c r="I15" s="23"/>
+      <c r="J15" s="26" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:253" ht="30">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="C16" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11" t="s">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="27"/>
-      <c r="J16" s="30" t="s">
-        <v>85</v>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="26" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
       <c r="A17" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="G17" s="11"/>
-      <c r="H17" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" s="27"/>
-      <c r="J17" s="30" t="s">
-        <v>88</v>
+      <c r="H17" s="11"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="26" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
@@ -2437,92 +2430,92 @@
         <v>41</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>62</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="H18" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>91</v>
+        <v>41</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>80</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11" t="s">
-        <v>92</v>
+      <c r="I19" s="23"/>
+      <c r="J19" s="26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" customHeight="1">
-      <c r="A20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="11" t="s">
+      <c r="A20" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
       <c r="J20" s="11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="45">
-      <c r="A21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="11" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="30">
@@ -2530,10 +2523,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>87</v>
@@ -2544,216 +2537,216 @@
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11" t="s">
-        <v>97</v>
+      <c r="I22" s="23"/>
+      <c r="J22" s="26" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="B23" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11" t="s">
+      <c r="E24" s="41"/>
+      <c r="F24" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30">
-      <c r="A24" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45">
+      <c r="A25" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11" t="s">
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="45">
+      <c r="A26" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30">
+      <c r="A27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45">
+      <c r="A28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="45">
-      <c r="A25" s="11" t="s">
+      <c r="D28" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E25" s="11" t="s">
+      <c r="C29" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30">
-      <c r="A26" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="30">
-      <c r="A27" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
-      <c r="A29" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="K29"/>
     </row>
     <row r="30" spans="1:11" ht="30">
       <c r="A30" s="20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="20"/>
+        <v>87</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="F30" s="20"/>
-      <c r="G30" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="G30" s="20"/>
       <c r="H30" s="20"/>
       <c r="I30" s="20"/>
       <c r="J30" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>62</v>
@@ -2763,46 +2756,46 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30">
-      <c r="A32" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30.75" thickBot="1">
+      <c r="A32" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22" t="s">
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A33" s="34" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="16" t="s">
@@ -2811,11 +2804,11 @@
       <c r="B34" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="16" t="s">
         <v>122</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>123</v>
       </c>
       <c r="E34" s="16"/>
       <c r="F34" s="16"/>
@@ -2825,7 +2818,7 @@
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
       <c r="J34" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -2835,11 +2828,11 @@
       <c r="B35" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="24" t="s">
-        <v>125</v>
+      <c r="C35" s="43" t="s">
+        <v>124</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -2849,21 +2842,21 @@
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="26.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30">
       <c r="A36" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2873,7 +2866,7 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2883,11 +2876,11 @@
       <c r="B37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="24" t="s">
-        <v>130</v>
+      <c r="C37" s="43" t="s">
+        <v>129</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -2897,22 +2890,22 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="34" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
     </row>
     <row r="39" spans="1:10" ht="30">
       <c r="A39" s="16" t="s">
@@ -2922,10 +2915,10 @@
         <v>22</v>
       </c>
       <c r="C39" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="11" t="s">
@@ -2935,7 +2928,7 @@
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
       <c r="J39" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="30">
@@ -2946,10 +2939,10 @@
         <v>22</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11" t="s">
@@ -2959,7 +2952,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30">
@@ -2970,10 +2963,10 @@
         <v>22</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11" t="s">
@@ -2983,22 +2976,22 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="A42" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10" ht="45">
       <c r="A43" s="16" t="s">
@@ -3008,7 +3001,7 @@
         <v>26</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>61</v>
@@ -3021,22 +3014,22 @@
       <c r="H43" s="11"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="A44" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
     </row>
     <row r="45" spans="1:10" ht="45">
       <c r="A45" s="16" t="s">
@@ -3046,7 +3039,7 @@
         <v>28</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>61</v>
@@ -3059,22 +3052,22 @@
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="A46" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10" ht="45">
       <c r="A47" s="16" t="s">
@@ -3084,7 +3077,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>61</v>
@@ -3097,809 +3090,809 @@
       <c r="H47" s="11"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="C48" s="26"/>
+      <c r="C48" s="22"/>
     </row>
     <row r="49" spans="3:3">
-      <c r="C49" s="26"/>
+      <c r="C49" s="22"/>
     </row>
     <row r="50" spans="3:3">
-      <c r="C50" s="26"/>
+      <c r="C50" s="22"/>
     </row>
     <row r="51" spans="3:3">
-      <c r="C51" s="26"/>
+      <c r="C51" s="22"/>
     </row>
     <row r="52" spans="3:3">
-      <c r="C52" s="26"/>
+      <c r="C52" s="22"/>
     </row>
     <row r="53" spans="3:3">
-      <c r="C53" s="26"/>
+      <c r="C53" s="22"/>
     </row>
     <row r="54" spans="3:3">
-      <c r="C54" s="26"/>
+      <c r="C54" s="22"/>
     </row>
     <row r="55" spans="3:3">
-      <c r="C55" s="26"/>
+      <c r="C55" s="22"/>
     </row>
     <row r="56" spans="3:3">
-      <c r="C56" s="26"/>
+      <c r="C56" s="22"/>
     </row>
     <row r="57" spans="3:3">
-      <c r="C57" s="26"/>
+      <c r="C57" s="22"/>
     </row>
     <row r="58" spans="3:3">
-      <c r="C58" s="26"/>
+      <c r="C58" s="22"/>
     </row>
     <row r="59" spans="3:3">
-      <c r="C59" s="26"/>
+      <c r="C59" s="22"/>
     </row>
     <row r="60" spans="3:3">
-      <c r="C60" s="26"/>
+      <c r="C60" s="22"/>
     </row>
     <row r="61" spans="3:3">
-      <c r="C61" s="26"/>
+      <c r="C61" s="22"/>
     </row>
     <row r="62" spans="3:3">
-      <c r="C62" s="26"/>
+      <c r="C62" s="22"/>
     </row>
     <row r="63" spans="3:3">
-      <c r="C63" s="26"/>
+      <c r="C63" s="22"/>
     </row>
     <row r="64" spans="3:3">
-      <c r="C64" s="26"/>
+      <c r="C64" s="22"/>
     </row>
     <row r="65" spans="3:3">
-      <c r="C65" s="26"/>
+      <c r="C65" s="22"/>
     </row>
     <row r="66" spans="3:3">
-      <c r="C66" s="26"/>
+      <c r="C66" s="22"/>
     </row>
     <row r="67" spans="3:3">
-      <c r="C67" s="26"/>
+      <c r="C67" s="22"/>
     </row>
     <row r="68" spans="3:3">
-      <c r="C68" s="26"/>
+      <c r="C68" s="22"/>
     </row>
     <row r="69" spans="3:3">
-      <c r="C69" s="26"/>
+      <c r="C69" s="22"/>
     </row>
     <row r="70" spans="3:3">
-      <c r="C70" s="26"/>
+      <c r="C70" s="22"/>
     </row>
     <row r="71" spans="3:3">
-      <c r="C71" s="26"/>
+      <c r="C71" s="22"/>
     </row>
     <row r="72" spans="3:3">
-      <c r="C72" s="26"/>
+      <c r="C72" s="22"/>
     </row>
     <row r="73" spans="3:3">
-      <c r="C73" s="26"/>
+      <c r="C73" s="22"/>
     </row>
     <row r="74" spans="3:3">
-      <c r="C74" s="26"/>
+      <c r="C74" s="22"/>
     </row>
     <row r="75" spans="3:3">
-      <c r="C75" s="26"/>
+      <c r="C75" s="22"/>
     </row>
     <row r="76" spans="3:3">
-      <c r="C76" s="26"/>
+      <c r="C76" s="22"/>
     </row>
     <row r="77" spans="3:3">
-      <c r="C77" s="26"/>
+      <c r="C77" s="22"/>
     </row>
     <row r="78" spans="3:3">
-      <c r="C78" s="26"/>
+      <c r="C78" s="22"/>
     </row>
     <row r="79" spans="3:3">
-      <c r="C79" s="26"/>
+      <c r="C79" s="22"/>
     </row>
     <row r="80" spans="3:3">
-      <c r="C80" s="26"/>
+      <c r="C80" s="22"/>
     </row>
     <row r="81" spans="3:3">
-      <c r="C81" s="26"/>
+      <c r="C81" s="22"/>
     </row>
     <row r="82" spans="3:3">
-      <c r="C82" s="26"/>
+      <c r="C82" s="22"/>
     </row>
     <row r="83" spans="3:3">
-      <c r="C83" s="26"/>
+      <c r="C83" s="22"/>
     </row>
     <row r="84" spans="3:3">
-      <c r="C84" s="26"/>
+      <c r="C84" s="22"/>
     </row>
     <row r="85" spans="3:3">
-      <c r="C85" s="26"/>
+      <c r="C85" s="22"/>
     </row>
     <row r="86" spans="3:3">
-      <c r="C86" s="26"/>
+      <c r="C86" s="22"/>
     </row>
     <row r="87" spans="3:3">
-      <c r="C87" s="26"/>
+      <c r="C87" s="22"/>
     </row>
     <row r="88" spans="3:3">
-      <c r="C88" s="26"/>
+      <c r="C88" s="22"/>
     </row>
     <row r="89" spans="3:3">
-      <c r="C89" s="26"/>
+      <c r="C89" s="22"/>
     </row>
     <row r="90" spans="3:3">
-      <c r="C90" s="26"/>
+      <c r="C90" s="22"/>
     </row>
     <row r="91" spans="3:3">
-      <c r="C91" s="26"/>
+      <c r="C91" s="22"/>
     </row>
     <row r="92" spans="3:3">
-      <c r="C92" s="26"/>
+      <c r="C92" s="22"/>
     </row>
     <row r="93" spans="3:3">
-      <c r="C93" s="26"/>
+      <c r="C93" s="22"/>
     </row>
     <row r="94" spans="3:3">
-      <c r="C94" s="26"/>
+      <c r="C94" s="22"/>
     </row>
     <row r="95" spans="3:3">
-      <c r="C95" s="26"/>
+      <c r="C95" s="22"/>
     </row>
     <row r="96" spans="3:3">
-      <c r="C96" s="26"/>
+      <c r="C96" s="22"/>
     </row>
     <row r="97" spans="3:3">
-      <c r="C97" s="26"/>
+      <c r="C97" s="22"/>
     </row>
     <row r="98" spans="3:3">
-      <c r="C98" s="26"/>
+      <c r="C98" s="22"/>
     </row>
     <row r="99" spans="3:3">
-      <c r="C99" s="26"/>
+      <c r="C99" s="22"/>
     </row>
     <row r="100" spans="3:3">
-      <c r="C100" s="26"/>
+      <c r="C100" s="22"/>
     </row>
     <row r="101" spans="3:3">
-      <c r="C101" s="26"/>
+      <c r="C101" s="22"/>
     </row>
     <row r="102" spans="3:3">
-      <c r="C102" s="26"/>
+      <c r="C102" s="22"/>
     </row>
     <row r="103" spans="3:3">
-      <c r="C103" s="26"/>
+      <c r="C103" s="22"/>
     </row>
     <row r="104" spans="3:3">
-      <c r="C104" s="26"/>
+      <c r="C104" s="22"/>
     </row>
     <row r="105" spans="3:3">
-      <c r="C105" s="26"/>
+      <c r="C105" s="22"/>
     </row>
     <row r="106" spans="3:3">
-      <c r="C106" s="26"/>
+      <c r="C106" s="22"/>
     </row>
     <row r="107" spans="3:3">
-      <c r="C107" s="26"/>
+      <c r="C107" s="22"/>
     </row>
     <row r="108" spans="3:3">
-      <c r="C108" s="26"/>
+      <c r="C108" s="22"/>
     </row>
     <row r="109" spans="3:3">
-      <c r="C109" s="26"/>
+      <c r="C109" s="22"/>
     </row>
     <row r="110" spans="3:3">
-      <c r="C110" s="26"/>
+      <c r="C110" s="22"/>
     </row>
     <row r="111" spans="3:3">
-      <c r="C111" s="26"/>
+      <c r="C111" s="22"/>
     </row>
     <row r="112" spans="3:3">
-      <c r="C112" s="26"/>
+      <c r="C112" s="22"/>
     </row>
     <row r="113" spans="3:3">
-      <c r="C113" s="26"/>
+      <c r="C113" s="22"/>
     </row>
     <row r="114" spans="3:3">
-      <c r="C114" s="26"/>
+      <c r="C114" s="22"/>
     </row>
     <row r="115" spans="3:3">
-      <c r="C115" s="26"/>
+      <c r="C115" s="22"/>
     </row>
     <row r="116" spans="3:3">
-      <c r="C116" s="26"/>
+      <c r="C116" s="22"/>
     </row>
     <row r="117" spans="3:3">
-      <c r="C117" s="26"/>
+      <c r="C117" s="22"/>
     </row>
     <row r="118" spans="3:3">
-      <c r="C118" s="26"/>
+      <c r="C118" s="22"/>
     </row>
     <row r="119" spans="3:3">
-      <c r="C119" s="26"/>
+      <c r="C119" s="22"/>
     </row>
     <row r="120" spans="3:3">
-      <c r="C120" s="26"/>
+      <c r="C120" s="22"/>
     </row>
     <row r="121" spans="3:3">
-      <c r="C121" s="26"/>
+      <c r="C121" s="22"/>
     </row>
     <row r="122" spans="3:3">
-      <c r="C122" s="26"/>
+      <c r="C122" s="22"/>
     </row>
     <row r="123" spans="3:3">
-      <c r="C123" s="26"/>
+      <c r="C123" s="22"/>
     </row>
     <row r="124" spans="3:3">
-      <c r="C124" s="26"/>
+      <c r="C124" s="22"/>
     </row>
     <row r="125" spans="3:3">
-      <c r="C125" s="26"/>
+      <c r="C125" s="22"/>
     </row>
     <row r="126" spans="3:3">
-      <c r="C126" s="26"/>
+      <c r="C126" s="22"/>
     </row>
     <row r="127" spans="3:3">
-      <c r="C127" s="26"/>
+      <c r="C127" s="22"/>
     </row>
     <row r="128" spans="3:3">
-      <c r="C128" s="26"/>
+      <c r="C128" s="22"/>
     </row>
     <row r="129" spans="3:3">
-      <c r="C129" s="26"/>
+      <c r="C129" s="22"/>
     </row>
     <row r="130" spans="3:3">
-      <c r="C130" s="26"/>
+      <c r="C130" s="22"/>
     </row>
     <row r="131" spans="3:3">
-      <c r="C131" s="26"/>
+      <c r="C131" s="22"/>
     </row>
     <row r="132" spans="3:3">
-      <c r="C132" s="26"/>
+      <c r="C132" s="22"/>
     </row>
     <row r="133" spans="3:3">
-      <c r="C133" s="26"/>
+      <c r="C133" s="22"/>
     </row>
     <row r="134" spans="3:3">
-      <c r="C134" s="26"/>
+      <c r="C134" s="22"/>
     </row>
     <row r="135" spans="3:3">
-      <c r="C135" s="26"/>
+      <c r="C135" s="22"/>
     </row>
     <row r="136" spans="3:3">
-      <c r="C136" s="26"/>
+      <c r="C136" s="22"/>
     </row>
     <row r="137" spans="3:3">
-      <c r="C137" s="26"/>
+      <c r="C137" s="22"/>
     </row>
     <row r="138" spans="3:3">
-      <c r="C138" s="26"/>
+      <c r="C138" s="22"/>
     </row>
     <row r="139" spans="3:3">
-      <c r="C139" s="26"/>
+      <c r="C139" s="22"/>
     </row>
     <row r="140" spans="3:3">
-      <c r="C140" s="26"/>
+      <c r="C140" s="22"/>
     </row>
     <row r="141" spans="3:3">
-      <c r="C141" s="26"/>
+      <c r="C141" s="22"/>
     </row>
     <row r="142" spans="3:3">
-      <c r="C142" s="26"/>
+      <c r="C142" s="22"/>
     </row>
     <row r="143" spans="3:3">
-      <c r="C143" s="26"/>
+      <c r="C143" s="22"/>
     </row>
     <row r="144" spans="3:3">
-      <c r="C144" s="26"/>
+      <c r="C144" s="22"/>
     </row>
     <row r="145" spans="3:3">
-      <c r="C145" s="26"/>
+      <c r="C145" s="22"/>
     </row>
     <row r="146" spans="3:3">
-      <c r="C146" s="26"/>
+      <c r="C146" s="22"/>
     </row>
     <row r="147" spans="3:3">
-      <c r="C147" s="26"/>
+      <c r="C147" s="22"/>
     </row>
     <row r="148" spans="3:3">
-      <c r="C148" s="26"/>
+      <c r="C148" s="22"/>
     </row>
     <row r="149" spans="3:3">
-      <c r="C149" s="26"/>
+      <c r="C149" s="22"/>
     </row>
     <row r="150" spans="3:3">
-      <c r="C150" s="26"/>
+      <c r="C150" s="22"/>
     </row>
     <row r="151" spans="3:3">
-      <c r="C151" s="26"/>
+      <c r="C151" s="22"/>
     </row>
     <row r="152" spans="3:3">
-      <c r="C152" s="26"/>
+      <c r="C152" s="22"/>
     </row>
     <row r="153" spans="3:3">
-      <c r="C153" s="26"/>
+      <c r="C153" s="22"/>
     </row>
     <row r="154" spans="3:3">
-      <c r="C154" s="26"/>
+      <c r="C154" s="22"/>
     </row>
     <row r="155" spans="3:3">
-      <c r="C155" s="26"/>
+      <c r="C155" s="22"/>
     </row>
     <row r="156" spans="3:3">
-      <c r="C156" s="26"/>
+      <c r="C156" s="22"/>
     </row>
     <row r="157" spans="3:3">
-      <c r="C157" s="26"/>
+      <c r="C157" s="22"/>
     </row>
     <row r="158" spans="3:3">
-      <c r="C158" s="26"/>
+      <c r="C158" s="22"/>
     </row>
     <row r="159" spans="3:3">
-      <c r="C159" s="26"/>
+      <c r="C159" s="22"/>
     </row>
     <row r="160" spans="3:3">
-      <c r="C160" s="26"/>
+      <c r="C160" s="22"/>
     </row>
     <row r="161" spans="3:3">
-      <c r="C161" s="26"/>
+      <c r="C161" s="22"/>
     </row>
     <row r="162" spans="3:3">
-      <c r="C162" s="26"/>
+      <c r="C162" s="22"/>
     </row>
     <row r="163" spans="3:3">
-      <c r="C163" s="26"/>
+      <c r="C163" s="22"/>
     </row>
     <row r="164" spans="3:3">
-      <c r="C164" s="26"/>
+      <c r="C164" s="22"/>
     </row>
     <row r="165" spans="3:3">
-      <c r="C165" s="26"/>
+      <c r="C165" s="22"/>
     </row>
     <row r="166" spans="3:3">
-      <c r="C166" s="26"/>
+      <c r="C166" s="22"/>
     </row>
     <row r="167" spans="3:3">
-      <c r="C167" s="26"/>
+      <c r="C167" s="22"/>
     </row>
     <row r="168" spans="3:3">
-      <c r="C168" s="26"/>
+      <c r="C168" s="22"/>
     </row>
     <row r="169" spans="3:3">
-      <c r="C169" s="26"/>
+      <c r="C169" s="22"/>
     </row>
     <row r="170" spans="3:3">
-      <c r="C170" s="26"/>
+      <c r="C170" s="22"/>
     </row>
     <row r="171" spans="3:3">
-      <c r="C171" s="26"/>
+      <c r="C171" s="22"/>
     </row>
     <row r="172" spans="3:3">
-      <c r="C172" s="26"/>
+      <c r="C172" s="22"/>
     </row>
     <row r="173" spans="3:3">
-      <c r="C173" s="26"/>
+      <c r="C173" s="22"/>
     </row>
     <row r="174" spans="3:3">
-      <c r="C174" s="26"/>
+      <c r="C174" s="22"/>
     </row>
     <row r="175" spans="3:3">
-      <c r="C175" s="26"/>
+      <c r="C175" s="22"/>
     </row>
     <row r="176" spans="3:3">
-      <c r="C176" s="26"/>
+      <c r="C176" s="22"/>
     </row>
     <row r="177" spans="3:3">
-      <c r="C177" s="26"/>
+      <c r="C177" s="22"/>
     </row>
     <row r="178" spans="3:3">
-      <c r="C178" s="26"/>
+      <c r="C178" s="22"/>
     </row>
     <row r="179" spans="3:3">
-      <c r="C179" s="26"/>
+      <c r="C179" s="22"/>
     </row>
     <row r="180" spans="3:3">
-      <c r="C180" s="26"/>
+      <c r="C180" s="22"/>
     </row>
     <row r="181" spans="3:3">
-      <c r="C181" s="26"/>
+      <c r="C181" s="22"/>
     </row>
     <row r="182" spans="3:3">
-      <c r="C182" s="26"/>
+      <c r="C182" s="22"/>
     </row>
     <row r="183" spans="3:3">
-      <c r="C183" s="26"/>
+      <c r="C183" s="22"/>
     </row>
     <row r="184" spans="3:3">
-      <c r="C184" s="26"/>
+      <c r="C184" s="22"/>
     </row>
     <row r="185" spans="3:3">
-      <c r="C185" s="26"/>
+      <c r="C185" s="22"/>
     </row>
     <row r="186" spans="3:3">
-      <c r="C186" s="26"/>
+      <c r="C186" s="22"/>
     </row>
     <row r="187" spans="3:3">
-      <c r="C187" s="26"/>
+      <c r="C187" s="22"/>
     </row>
     <row r="188" spans="3:3">
-      <c r="C188" s="26"/>
+      <c r="C188" s="22"/>
     </row>
     <row r="189" spans="3:3">
-      <c r="C189" s="26"/>
+      <c r="C189" s="22"/>
     </row>
     <row r="190" spans="3:3">
-      <c r="C190" s="26"/>
+      <c r="C190" s="22"/>
     </row>
     <row r="191" spans="3:3">
-      <c r="C191" s="26"/>
+      <c r="C191" s="22"/>
     </row>
     <row r="192" spans="3:3">
-      <c r="C192" s="26"/>
+      <c r="C192" s="22"/>
     </row>
     <row r="193" spans="3:3">
-      <c r="C193" s="26"/>
+      <c r="C193" s="22"/>
     </row>
     <row r="194" spans="3:3">
-      <c r="C194" s="26"/>
+      <c r="C194" s="22"/>
     </row>
     <row r="195" spans="3:3">
-      <c r="C195" s="26"/>
+      <c r="C195" s="22"/>
     </row>
     <row r="196" spans="3:3">
-      <c r="C196" s="26"/>
+      <c r="C196" s="22"/>
     </row>
     <row r="197" spans="3:3">
-      <c r="C197" s="26"/>
+      <c r="C197" s="22"/>
     </row>
     <row r="198" spans="3:3">
-      <c r="C198" s="26"/>
+      <c r="C198" s="22"/>
     </row>
     <row r="199" spans="3:3">
-      <c r="C199" s="26"/>
+      <c r="C199" s="22"/>
     </row>
     <row r="200" spans="3:3">
-      <c r="C200" s="26"/>
+      <c r="C200" s="22"/>
     </row>
     <row r="201" spans="3:3">
-      <c r="C201" s="26"/>
+      <c r="C201" s="22"/>
     </row>
     <row r="202" spans="3:3">
-      <c r="C202" s="26"/>
+      <c r="C202" s="22"/>
     </row>
     <row r="203" spans="3:3">
-      <c r="C203" s="26"/>
+      <c r="C203" s="22"/>
     </row>
     <row r="204" spans="3:3">
-      <c r="C204" s="26"/>
+      <c r="C204" s="22"/>
     </row>
     <row r="205" spans="3:3">
-      <c r="C205" s="26"/>
+      <c r="C205" s="22"/>
     </row>
     <row r="206" spans="3:3">
-      <c r="C206" s="26"/>
+      <c r="C206" s="22"/>
     </row>
     <row r="207" spans="3:3">
-      <c r="C207" s="26"/>
+      <c r="C207" s="22"/>
     </row>
     <row r="208" spans="3:3">
-      <c r="C208" s="26"/>
+      <c r="C208" s="22"/>
     </row>
     <row r="209" spans="3:3">
-      <c r="C209" s="26"/>
+      <c r="C209" s="22"/>
     </row>
     <row r="210" spans="3:3">
-      <c r="C210" s="26"/>
+      <c r="C210" s="22"/>
     </row>
     <row r="211" spans="3:3">
-      <c r="C211" s="26"/>
+      <c r="C211" s="22"/>
     </row>
     <row r="212" spans="3:3">
-      <c r="C212" s="26"/>
+      <c r="C212" s="22"/>
     </row>
     <row r="213" spans="3:3">
-      <c r="C213" s="26"/>
+      <c r="C213" s="22"/>
     </row>
     <row r="214" spans="3:3">
-      <c r="C214" s="26"/>
+      <c r="C214" s="22"/>
     </row>
     <row r="215" spans="3:3">
-      <c r="C215" s="26"/>
+      <c r="C215" s="22"/>
     </row>
     <row r="216" spans="3:3">
-      <c r="C216" s="26"/>
+      <c r="C216" s="22"/>
     </row>
     <row r="217" spans="3:3">
-      <c r="C217" s="26"/>
+      <c r="C217" s="22"/>
     </row>
     <row r="218" spans="3:3">
-      <c r="C218" s="26"/>
+      <c r="C218" s="22"/>
     </row>
     <row r="219" spans="3:3">
-      <c r="C219" s="26"/>
+      <c r="C219" s="22"/>
     </row>
     <row r="220" spans="3:3">
-      <c r="C220" s="26"/>
+      <c r="C220" s="22"/>
     </row>
     <row r="221" spans="3:3">
-      <c r="C221" s="26"/>
+      <c r="C221" s="22"/>
     </row>
     <row r="222" spans="3:3">
-      <c r="C222" s="26"/>
+      <c r="C222" s="22"/>
     </row>
     <row r="223" spans="3:3">
-      <c r="C223" s="26"/>
+      <c r="C223" s="22"/>
     </row>
     <row r="224" spans="3:3">
-      <c r="C224" s="26"/>
+      <c r="C224" s="22"/>
     </row>
     <row r="225" spans="3:3">
-      <c r="C225" s="26"/>
+      <c r="C225" s="22"/>
     </row>
     <row r="226" spans="3:3">
-      <c r="C226" s="26"/>
+      <c r="C226" s="22"/>
     </row>
     <row r="227" spans="3:3">
-      <c r="C227" s="26"/>
+      <c r="C227" s="22"/>
     </row>
     <row r="228" spans="3:3">
-      <c r="C228" s="26"/>
+      <c r="C228" s="22"/>
     </row>
     <row r="229" spans="3:3">
-      <c r="C229" s="26"/>
+      <c r="C229" s="22"/>
     </row>
     <row r="230" spans="3:3">
-      <c r="C230" s="26"/>
+      <c r="C230" s="22"/>
     </row>
     <row r="231" spans="3:3">
-      <c r="C231" s="26"/>
+      <c r="C231" s="22"/>
     </row>
     <row r="232" spans="3:3">
-      <c r="C232" s="26"/>
+      <c r="C232" s="22"/>
     </row>
     <row r="233" spans="3:3">
-      <c r="C233" s="26"/>
+      <c r="C233" s="22"/>
     </row>
     <row r="234" spans="3:3">
-      <c r="C234" s="26"/>
+      <c r="C234" s="22"/>
     </row>
     <row r="235" spans="3:3">
-      <c r="C235" s="26"/>
+      <c r="C235" s="22"/>
     </row>
     <row r="236" spans="3:3">
-      <c r="C236" s="26"/>
+      <c r="C236" s="22"/>
     </row>
     <row r="237" spans="3:3">
-      <c r="C237" s="26"/>
+      <c r="C237" s="22"/>
     </row>
     <row r="238" spans="3:3">
-      <c r="C238" s="26"/>
+      <c r="C238" s="22"/>
     </row>
     <row r="239" spans="3:3">
-      <c r="C239" s="26"/>
+      <c r="C239" s="22"/>
     </row>
     <row r="240" spans="3:3">
-      <c r="C240" s="26"/>
+      <c r="C240" s="22"/>
     </row>
     <row r="241" spans="3:3">
-      <c r="C241" s="26"/>
+      <c r="C241" s="22"/>
     </row>
     <row r="242" spans="3:3">
-      <c r="C242" s="26"/>
+      <c r="C242" s="22"/>
     </row>
     <row r="243" spans="3:3">
-      <c r="C243" s="26"/>
+      <c r="C243" s="22"/>
     </row>
     <row r="244" spans="3:3">
-      <c r="C244" s="26"/>
+      <c r="C244" s="22"/>
     </row>
     <row r="245" spans="3:3">
-      <c r="C245" s="26"/>
+      <c r="C245" s="22"/>
     </row>
     <row r="246" spans="3:3">
-      <c r="C246" s="26"/>
+      <c r="C246" s="22"/>
     </row>
     <row r="247" spans="3:3">
-      <c r="C247" s="26"/>
+      <c r="C247" s="22"/>
     </row>
     <row r="248" spans="3:3">
-      <c r="C248" s="26"/>
+      <c r="C248" s="22"/>
     </row>
     <row r="249" spans="3:3">
-      <c r="C249" s="26"/>
+      <c r="C249" s="22"/>
     </row>
     <row r="250" spans="3:3">
-      <c r="C250" s="26"/>
+      <c r="C250" s="22"/>
     </row>
     <row r="251" spans="3:3">
-      <c r="C251" s="26"/>
+      <c r="C251" s="22"/>
     </row>
     <row r="252" spans="3:3">
-      <c r="C252" s="26"/>
+      <c r="C252" s="22"/>
     </row>
     <row r="253" spans="3:3">
-      <c r="C253" s="26"/>
+      <c r="C253" s="22"/>
     </row>
     <row r="254" spans="3:3">
-      <c r="C254" s="26"/>
+      <c r="C254" s="22"/>
     </row>
     <row r="255" spans="3:3">
-      <c r="C255" s="26"/>
+      <c r="C255" s="22"/>
     </row>
     <row r="256" spans="3:3">
-      <c r="C256" s="26"/>
+      <c r="C256" s="22"/>
     </row>
     <row r="257" spans="3:3">
-      <c r="C257" s="26"/>
+      <c r="C257" s="22"/>
     </row>
     <row r="258" spans="3:3">
-      <c r="C258" s="26"/>
+      <c r="C258" s="22"/>
     </row>
     <row r="259" spans="3:3">
-      <c r="C259" s="26"/>
+      <c r="C259" s="22"/>
     </row>
     <row r="260" spans="3:3">
-      <c r="C260" s="26"/>
+      <c r="C260" s="22"/>
     </row>
     <row r="261" spans="3:3">
-      <c r="C261" s="26"/>
+      <c r="C261" s="22"/>
     </row>
     <row r="262" spans="3:3">
-      <c r="C262" s="26"/>
+      <c r="C262" s="22"/>
     </row>
     <row r="263" spans="3:3">
-      <c r="C263" s="26"/>
+      <c r="C263" s="22"/>
     </row>
     <row r="264" spans="3:3">
-      <c r="C264" s="26"/>
+      <c r="C264" s="22"/>
     </row>
     <row r="265" spans="3:3">
-      <c r="C265" s="26"/>
+      <c r="C265" s="22"/>
     </row>
     <row r="266" spans="3:3">
-      <c r="C266" s="26"/>
+      <c r="C266" s="22"/>
     </row>
     <row r="267" spans="3:3">
-      <c r="C267" s="26"/>
+      <c r="C267" s="22"/>
     </row>
     <row r="268" spans="3:3">
-      <c r="C268" s="26"/>
+      <c r="C268" s="22"/>
     </row>
     <row r="269" spans="3:3">
-      <c r="C269" s="26"/>
+      <c r="C269" s="22"/>
     </row>
     <row r="270" spans="3:3">
-      <c r="C270" s="26"/>
+      <c r="C270" s="22"/>
     </row>
     <row r="271" spans="3:3">
-      <c r="C271" s="26"/>
+      <c r="C271" s="22"/>
     </row>
     <row r="272" spans="3:3">
-      <c r="C272" s="26"/>
+      <c r="C272" s="22"/>
     </row>
     <row r="273" spans="3:3">
-      <c r="C273" s="26"/>
+      <c r="C273" s="22"/>
     </row>
     <row r="274" spans="3:3">
-      <c r="C274" s="26"/>
+      <c r="C274" s="22"/>
     </row>
     <row r="275" spans="3:3">
-      <c r="C275" s="26"/>
+      <c r="C275" s="22"/>
     </row>
     <row r="276" spans="3:3">
-      <c r="C276" s="26"/>
+      <c r="C276" s="22"/>
     </row>
     <row r="277" spans="3:3">
-      <c r="C277" s="26"/>
+      <c r="C277" s="22"/>
     </row>
     <row r="278" spans="3:3">
-      <c r="C278" s="26"/>
+      <c r="C278" s="22"/>
     </row>
     <row r="279" spans="3:3">
-      <c r="C279" s="26"/>
+      <c r="C279" s="22"/>
     </row>
     <row r="280" spans="3:3">
-      <c r="C280" s="26"/>
+      <c r="C280" s="22"/>
     </row>
     <row r="281" spans="3:3">
-      <c r="C281" s="26"/>
+      <c r="C281" s="22"/>
     </row>
     <row r="282" spans="3:3">
-      <c r="C282" s="26"/>
+      <c r="C282" s="22"/>
     </row>
     <row r="283" spans="3:3">
-      <c r="C283" s="26"/>
+      <c r="C283" s="22"/>
     </row>
     <row r="284" spans="3:3">
-      <c r="C284" s="26"/>
+      <c r="C284" s="22"/>
     </row>
     <row r="285" spans="3:3">
-      <c r="C285" s="26"/>
+      <c r="C285" s="22"/>
     </row>
     <row r="286" spans="3:3">
-      <c r="C286" s="26"/>
+      <c r="C286" s="22"/>
     </row>
     <row r="287" spans="3:3">
-      <c r="C287" s="26"/>
+      <c r="C287" s="22"/>
     </row>
     <row r="288" spans="3:3">
-      <c r="C288" s="26"/>
+      <c r="C288" s="22"/>
     </row>
     <row r="289" spans="3:3">
-      <c r="C289" s="26"/>
+      <c r="C289" s="22"/>
     </row>
     <row r="290" spans="3:3">
-      <c r="C290" s="26"/>
+      <c r="C290" s="22"/>
     </row>
     <row r="291" spans="3:3">
-      <c r="C291" s="26"/>
+      <c r="C291" s="22"/>
     </row>
     <row r="292" spans="3:3">
-      <c r="C292" s="26"/>
+      <c r="C292" s="22"/>
     </row>
     <row r="293" spans="3:3">
-      <c r="C293" s="26"/>
+      <c r="C293" s="22"/>
     </row>
     <row r="294" spans="3:3">
-      <c r="C294" s="26"/>
+      <c r="C294" s="22"/>
     </row>
     <row r="295" spans="3:3">
-      <c r="C295" s="26"/>
+      <c r="C295" s="22"/>
     </row>
     <row r="296" spans="3:3">
-      <c r="C296" s="26"/>
+      <c r="C296" s="22"/>
     </row>
     <row r="297" spans="3:3">
-      <c r="C297" s="26"/>
+      <c r="C297" s="22"/>
     </row>
     <row r="298" spans="3:3">
-      <c r="C298" s="26"/>
+      <c r="C298" s="22"/>
     </row>
     <row r="299" spans="3:3">
-      <c r="C299" s="26"/>
+      <c r="C299" s="22"/>
     </row>
     <row r="300" spans="3:3">
-      <c r="C300" s="26"/>
+      <c r="C300" s="22"/>
     </row>
     <row r="301" spans="3:3">
-      <c r="C301" s="26"/>
+      <c r="C301" s="22"/>
     </row>
     <row r="302" spans="3:3">
-      <c r="C302" s="26"/>
+      <c r="C302" s="22"/>
     </row>
     <row r="303" spans="3:3">
-      <c r="C303" s="26"/>
+      <c r="C303" s="22"/>
     </row>
     <row r="304" spans="3:3">
-      <c r="C304" s="26"/>
+      <c r="C304" s="22"/>
     </row>
     <row r="305" spans="3:3">
-      <c r="C305" s="26"/>
+      <c r="C305" s="22"/>
     </row>
     <row r="306" spans="3:3">
-      <c r="C306" s="26"/>
+      <c r="C306" s="22"/>
     </row>
     <row r="307" spans="3:3">
-      <c r="C307" s="26"/>
+      <c r="C307" s="22"/>
     </row>
     <row r="308" spans="3:3">
-      <c r="C308" s="26"/>
+      <c r="C308" s="22"/>
     </row>
     <row r="309" spans="3:3">
-      <c r="C309" s="26"/>
+      <c r="C309" s="22"/>
     </row>
     <row r="310" spans="3:3">
-      <c r="C310" s="26"/>
+      <c r="C310" s="22"/>
     </row>
     <row r="311" spans="3:3">
-      <c r="C311" s="26"/>
+      <c r="C311" s="22"/>
     </row>
     <row r="312" spans="3:3">
-      <c r="C312" s="26"/>
+      <c r="C312" s="22"/>
     </row>
     <row r="313" spans="3:3">
-      <c r="C313" s="26"/>
+      <c r="C313" s="22"/>
     </row>
     <row r="314" spans="3:3">
-      <c r="C314" s="26"/>
+      <c r="C314" s="22"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3919,7 +3912,7 @@
     <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -3938,14 +3931,14 @@
   </cols>
   <sheetData>
     <row r="29" spans="4:9">
-      <c r="D29" s="42" t="s">
-        <v>150</v>
-      </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
+      <c r="D29" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3973,14 +3966,14 @@
   </cols>
   <sheetData>
     <row r="40" spans="2:7">
-      <c r="B40" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="43"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
+      <c r="B40" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Final Version, Mark I
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -8,19 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="1" r:id="rId1"/>
-    <sheet name="Both Active" sheetId="2" r:id="rId2"/>
+    <sheet name="RVM" sheetId="2" r:id="rId2"/>
     <sheet name="Figure 1-Coordinate System" sheetId="3" r:id="rId3"/>
     <sheet name="Figure 2- NASA Gevs" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="__Anonymous_Sheet_DB__1">'Both Active'!$D$41</definedName>
+    <definedName name="__Anonymous_Sheet_DB__1">RVM!$D$42</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="160">
   <si>
     <t>Document Title</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>RCL-STR-RVM5</t>
-  </si>
-  <si>
-    <t>Center of gravity shall be located within a sphere of 2 cm of the geometric center</t>
   </si>
   <si>
     <t>RCL-STR-RVM2</t>
@@ -620,6 +617,18 @@
   </si>
   <si>
     <t xml:space="preserve">Individual CubeSat system shall achieve a local slew rate of less than 1 deg/s </t>
+  </si>
+  <si>
+    <t>Center of  gravity total CubeSat system shall be located within a sphere of 2 cm of the geometric center of the system</t>
+  </si>
+  <si>
+    <t>Center of  gravity of each CubeSat system shall be located within a sphere of 2 cm of the geometric center of said system</t>
+  </si>
+  <si>
+    <t>Attitude Determination and Control Requirement</t>
+  </si>
+  <si>
+    <t>RCL-STR-RVM16</t>
   </si>
 </sst>
 </file>
@@ -886,7 +895,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1007,6 +1016,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1956,10 +1968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IS314"/>
+  <dimension ref="A1:IS315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2068,7 +2080,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>64</v>
@@ -2081,7 +2093,7 @@
       </c>
       <c r="I5" s="24"/>
       <c r="J5" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M5" s="14"/>
       <c r="T5" s="15"/>
@@ -2141,7 +2153,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>64</v>
@@ -2154,7 +2166,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="23"/>
       <c r="J6" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:253" s="10" customFormat="1" ht="30">
@@ -2165,7 +2177,7 @@
         <v>41</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>64</v>
@@ -2189,7 +2201,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>61</v>
@@ -2202,7 +2214,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:253" ht="30">
@@ -2213,10 +2225,10 @@
         <v>39</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>100</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11" t="s">
@@ -2226,7 +2238,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:253">
@@ -2237,7 +2249,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>61</v>
@@ -2261,7 +2273,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>64</v>
@@ -2285,7 +2297,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>64</v>
@@ -2298,7 +2310,7 @@
       </c>
       <c r="I12" s="23"/>
       <c r="J12" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:253" ht="30">
@@ -2309,7 +2321,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>64</v>
@@ -2322,7 +2334,7 @@
       </c>
       <c r="I13" s="23"/>
       <c r="J13" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:253" ht="30">
@@ -2333,7 +2345,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>64</v>
@@ -2346,7 +2358,7 @@
       </c>
       <c r="I14" s="23"/>
       <c r="J14" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V14" s="25"/>
     </row>
@@ -2358,7 +2370,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>64</v>
@@ -2371,7 +2383,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="23"/>
       <c r="J15" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:253" ht="30">
@@ -2382,7 +2394,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>64</v>
@@ -2395,55 +2407,55 @@
       <c r="H16" s="16"/>
       <c r="I16" s="24"/>
       <c r="J16" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30">
-      <c r="A17" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11" t="s">
+      <c r="C17" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="23"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30">
       <c r="A18" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="G18" s="11"/>
-      <c r="H18" s="11" t="s">
-        <v>62</v>
-      </c>
+      <c r="H18" s="11"/>
       <c r="I18" s="23"/>
       <c r="J18" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30">
@@ -2454,7 +2466,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>64</v>
@@ -2467,34 +2479,34 @@
       </c>
       <c r="I19" s="23"/>
       <c r="J19" s="26" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1">
-      <c r="A20" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30">
+      <c r="I20" s="23"/>
+      <c r="J20" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" customHeight="1">
       <c r="A21" s="20" t="s">
         <v>14</v>
       </c>
@@ -2502,178 +2514,178 @@
         <v>33</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
       <c r="J21" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="30">
+      <c r="A22" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30">
+      <c r="A25" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="41" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
-      <c r="A22" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="C25" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30">
-      <c r="A24" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="D24" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="45">
-      <c r="A25" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
       <c r="I25" s="41"/>
       <c r="J25" s="41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="45">
+      <c r="A26" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45">
+      <c r="A27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="45">
-      <c r="A26" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="30">
-      <c r="A27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="45">
+    <row r="28" spans="1:11" ht="30">
       <c r="A28" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>103</v>
+        <v>94</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>62</v>
@@ -2683,10 +2695,10 @@
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="45">
       <c r="A29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2694,10 +2706,10 @@
         <v>45</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>62</v>
@@ -2707,33 +2719,33 @@
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K29"/>
+        <v>103</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="30">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="20" t="s">
+      <c r="C30" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
       <c r="J30" s="11" t="s">
-        <v>109</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="K30"/>
     </row>
     <row r="31" spans="1:11" ht="30">
       <c r="A31" s="20" t="s">
@@ -2743,10 +2755,10 @@
         <v>45</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>62</v>
@@ -2756,10 +2768,10 @@
       <c r="H31" s="20"/>
       <c r="I31" s="20"/>
       <c r="J31" s="11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30.75" thickBot="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="20" t="s">
         <v>12</v>
       </c>
@@ -2767,10 +2779,10 @@
         <v>45</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32" s="20" t="s">
         <v>62</v>
@@ -2780,83 +2792,83 @@
       <c r="H32" s="20"/>
       <c r="I32" s="20"/>
       <c r="J32" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A33" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="34"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="D34" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="30.75" thickBot="1">
+      <c r="A33" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16" t="s">
-        <v>123</v>
-      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A34" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="D35" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="16" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="30">
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="44" t="s">
-        <v>126</v>
+      <c r="C36" s="43" t="s">
+        <v>123</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -2866,21 +2878,21 @@
       <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30">
       <c r="A37" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="43" t="s">
-        <v>129</v>
+      <c r="C37" s="44" t="s">
+        <v>125</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -2890,46 +2902,46 @@
       <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="34" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-    </row>
-    <row r="39" spans="1:10" ht="30">
-      <c r="A39" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11" t="s">
-        <v>134</v>
-      </c>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10" ht="30">
       <c r="A40" s="16" t="s">
@@ -2939,10 +2951,10 @@
         <v>22</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11" t="s">
@@ -2952,7 +2964,7 @@
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
       <c r="J40" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30">
@@ -2962,11 +2974,11 @@
       <c r="B41" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>136</v>
+      <c r="C41" s="17" t="s">
+        <v>155</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11" t="s">
@@ -2976,125 +2988,146 @@
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30">
+      <c r="A42" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="34" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="34" t="s">
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+    </row>
+    <row r="44" spans="1:10" ht="45">
+      <c r="A44" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
-    </row>
-    <row r="43" spans="1:10" ht="45">
-      <c r="A43" s="16" t="s">
+      <c r="D44" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+    </row>
+    <row r="46" spans="1:10" ht="45">
+      <c r="A46" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D43" s="11" t="s">
+      <c r="B46" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11" t="s">
+      <c r="E46" s="11"/>
+      <c r="F46" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="34" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
-    </row>
-    <row r="45" spans="1:10" ht="45">
-      <c r="A45" s="16" t="s">
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+    </row>
+    <row r="48" spans="1:10" ht="45">
+      <c r="A48" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D45" s="11" t="s">
+      <c r="B48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11" t="s">
+      <c r="E48" s="11"/>
+      <c r="F48" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-    </row>
-    <row r="47" spans="1:10" ht="45">
-      <c r="A47" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="18" t="s">
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D47" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="C48" s="22"/>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" s="22"/>
@@ -3893,6 +3926,9 @@
     </row>
     <row r="314" spans="3:3">
       <c r="C314" s="22"/>
+    </row>
+    <row r="315" spans="3:3">
+      <c r="C315" s="22"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3900,13 +3936,13 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A47:J47"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A44:J44"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="A45:J45"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -3932,7 +3968,7 @@
   <sheetData>
     <row r="29" spans="4:9">
       <c r="D29" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
@@ -3967,7 +4003,7 @@
   <sheetData>
     <row r="40" spans="2:7">
       <c r="B40" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="39"/>
       <c r="D40" s="39"/>

</xml_diff>

<commit_message>
Updated version with work assignment in place
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -1970,8 +1970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IS315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added format for the summaries that will work me
Cause Tom sucks
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -1970,8 +1970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IS315"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Requirements now have correct notation
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -13,14 +13,15 @@
     <sheet name="Figure 2- NASA Gevs" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="__Anonymous_Sheet_DB__1">RVM!$D$42</definedName>
+    <definedName name="__Anonymous_Sheet_DB__1">RVM!$D$45</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="166">
   <si>
     <t>Document Title</t>
   </si>
@@ -202,159 +203,49 @@
     <t>Stage 1: Pre-Mission Preliminary Design/Integration and Testing</t>
   </si>
   <si>
-    <t>The total CubeSat volume shall not exceed 6U</t>
-  </si>
-  <si>
     <t>Team Bravo RFP</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>RCL-STR-RVM1</t>
-  </si>
-  <si>
     <t>CubeSat Design Specification Rev 12</t>
   </si>
   <si>
-    <t>RCL-STR-RVM6</t>
-  </si>
-  <si>
-    <t>RCL-STR-RVM4</t>
-  </si>
-  <si>
-    <t>RCL-STR-RVM5</t>
-  </si>
-  <si>
-    <t>RCL-STR-RVM2</t>
-  </si>
-  <si>
     <t xml:space="preserve">No external components other than the CubeSat rails may make contact with the deployer </t>
   </si>
   <si>
-    <t>RCL-STR-RVM3</t>
-  </si>
-  <si>
     <t>No Protrusion shall extend beyond 6.5 mm normal to any external surface</t>
   </si>
   <si>
-    <t>RCL-STR-RVM7</t>
-  </si>
-  <si>
     <t>The deployer shall not be used to secure any CubeSat deployables</t>
   </si>
   <si>
-    <t>RCL-STR-RVM8</t>
-  </si>
-  <si>
-    <t>The CubeSat coordinate system shall be defined as specified in Figure 1</t>
-  </si>
-  <si>
-    <t>RCL-STR-RVM9</t>
-  </si>
-  <si>
     <t>The ends of the rails on the +Z/-Z faces shall have a minimum surface area of 6.5 mm x 6.5 mm</t>
   </si>
   <si>
-    <t>RCL-STR-RVM10</t>
-  </si>
-  <si>
-    <t>The +Y/-Y Faces of any CubeSat structure shall have a length of 100 mm</t>
-  </si>
-  <si>
-    <t>RCL-STR-RVM11</t>
-  </si>
-  <si>
-    <r>
-      <t>All materials used in the CubeSat shall have a Total Mass Loss of less than 1.0% (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>List of Low Out-gassing Materials available at outgassing.nasa.gov</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>RCL-STR-RVM12</t>
-  </si>
-  <si>
-    <t>All materials used in the CubeSat shall have a Collected Volatile Condensable material of less than 0.1%</t>
-  </si>
-  <si>
-    <t>RCL-STR-RVM13</t>
-  </si>
-  <si>
     <t>Low friction, 2D testing of the CubeSat system release mechanism shall be conducted</t>
   </si>
   <si>
     <t>Environmental Testing Requirements</t>
   </si>
   <si>
-    <t>RCL-STR-RVM14</t>
-  </si>
-  <si>
     <t>CubeSat system shall be conjoined before launch vehicle integration</t>
   </si>
   <si>
-    <t>RCL-STR-RVM15</t>
-  </si>
-  <si>
     <t>Pressure Vessels shall have a factor of safely no less than 4</t>
   </si>
   <si>
-    <t>RCL-PRP-RVM1</t>
-  </si>
-  <si>
-    <t>RCL-PRP-RVM2</t>
-  </si>
-  <si>
-    <t>RCL-PRP-RVM3</t>
-  </si>
-  <si>
     <t>Low friction, 2D dynamic thrust testing shall be conducted on the propulsion system</t>
   </si>
   <si>
-    <t>RCL-PRP-RVM4</t>
-  </si>
-  <si>
-    <t>CubeSat must be in orbit for at least 6 months</t>
-  </si>
-  <si>
-    <t>RCL-MOP-RVM1</t>
-  </si>
-  <si>
-    <t>CubeSat must deorbit within 25 years of being launched</t>
-  </si>
-  <si>
     <t>Process for Limiting Orbital Debris (NASA-STD-8719.14A)</t>
   </si>
   <si>
-    <t>RCL-MOP-RVM2</t>
-  </si>
-  <si>
     <t>CubeSat must survive Random Vibration Testing relative to the NASA GEVS Qualification Profile (Shown in Figure 2)</t>
   </si>
   <si>
     <t>General Environmental Verification Standard for GSFC Flight Programs and Projects (GSFC-STD-7000A)</t>
-  </si>
-  <si>
-    <t>RCL-TST-RVM1</t>
   </si>
   <si>
     <r>
@@ -385,45 +276,18 @@
     <t>Past ELaNa CubeSat-P-POD ICD's</t>
   </si>
   <si>
-    <t>RCL-TST-RVM2</t>
-  </si>
-  <si>
     <t>Full CubeSat System shall be able to execute all commands associated with its operation over RF</t>
   </si>
   <si>
-    <t>RCL-TST-RVM3</t>
-  </si>
-  <si>
     <t>Full CubeSat System shall be able to close a link with the SSRL Ground Station from a distance of at least 200 meters</t>
   </si>
   <si>
-    <t>RCL-TST-RVM4</t>
-  </si>
-  <si>
     <t>Full CubeSat System shall be able to document the functionality of each subsystem through the running of a full-functional test</t>
   </si>
   <si>
-    <t>RCL-TST-RVM5</t>
-  </si>
-  <si>
-    <t>The payload shall be capable of determining relative distance between two spacecraft</t>
-  </si>
-  <si>
-    <t>RCL-PLD-RVM1</t>
-  </si>
-  <si>
-    <t>CubeSat system shall be capable of recording relative displacement data</t>
-  </si>
-  <si>
-    <t>RCL-PLD-RVM2</t>
-  </si>
-  <si>
     <t>Thermal</t>
   </si>
   <si>
-    <t>RCL-THM-RVM1</t>
-  </si>
-  <si>
     <t>Stage 2: Post-launch Ejection</t>
   </si>
   <si>
@@ -433,91 +297,37 @@
     <t>LSP Requirement</t>
   </si>
   <si>
-    <t>RCL-PLE-RVM1</t>
-  </si>
-  <si>
     <t>CubeSat system shall not release deployables until ejection +45 minutes</t>
   </si>
   <si>
-    <t>RCL-PLE-RVM2</t>
-  </si>
-  <si>
     <t>CubeSat shall establish communication link between itself and SSRL ground station</t>
   </si>
   <si>
     <t>SSRL Requirement</t>
   </si>
   <si>
-    <t>RCL-PLE-RVM3</t>
-  </si>
-  <si>
     <t>CubeSat shall pass a health check initiated by SSRL</t>
   </si>
   <si>
-    <t>RCL-PLE-RVM4</t>
-  </si>
-  <si>
     <t>Stage 3: Separation &amp; Stabilization</t>
   </si>
   <si>
-    <t>CubeSat system shall be capable of separating from one another with a relative velocity no greater than 5 cm/s</t>
-  </si>
-  <si>
     <t>MATLAB Orbital Analysis</t>
   </si>
   <si>
-    <t>RCL-SS-RVM1</t>
-  </si>
-  <si>
-    <t>RCL-SS-RVM2</t>
-  </si>
-  <si>
-    <t>Individual CubeSat systems shall record relative displacement between each other</t>
-  </si>
-  <si>
-    <t>RCL-SS-RVM3</t>
-  </si>
-  <si>
     <t>Stage 4: StationKeeping</t>
   </si>
   <si>
-    <t xml:space="preserve">Individual CubeSat System shall be able to stationkeep within a 10-75 m sphere for at least 5 orbits relative to the other CubeSat system </t>
-  </si>
-  <si>
-    <t>RCL-SK-RVM1</t>
-  </si>
-  <si>
     <t>Stage 5: “Escape”</t>
   </si>
   <si>
-    <t>Individual CubeSat System shall be able to perform an “escape” maneuver that increases the final relative displacement from the other CubeSat system to at least 100 meters within 1 orbit</t>
-  </si>
-  <si>
-    <t>RCL-ESC-RVM1</t>
-  </si>
-  <si>
     <t>Stage 6: Rendezvous</t>
   </si>
   <si>
-    <t>Individual CubeSat System shall be able to a rendezvous by decreasing the final relative distance from the other CubeSat system to within 50 m for 5 orbits</t>
-  </si>
-  <si>
-    <t>RCL-RDZ-RVM1</t>
-  </si>
-  <si>
     <t>Figure 1- CubeSat Coordinate System</t>
   </si>
   <si>
     <t>Figure 2- NASA GEVS Random Vibration Profile</t>
-  </si>
-  <si>
-    <t>The total CubeSat mass shall not exceed 8.0 kg</t>
-  </si>
-  <si>
-    <t>The CubeSat shall incorporate a Remove Before Flight pin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The CubeSat shall incorporate a deployment switch </t>
   </si>
   <si>
     <r>
@@ -616,19 +426,228 @@
     <t>Reference Material (NAV Folder)</t>
   </si>
   <si>
-    <t xml:space="preserve">Individual CubeSat system shall achieve a local slew rate of less than 1 deg/s </t>
-  </si>
-  <si>
     <t>Center of  gravity total CubeSat system shall be located within a sphere of 2 cm of the geometric center of the system</t>
   </si>
   <si>
-    <t>Center of  gravity of each CubeSat system shall be located within a sphere of 2 cm of the geometric center of said system</t>
-  </si>
-  <si>
     <t>Attitude Determination and Control Requirement</t>
   </si>
   <si>
-    <t>RCL-STR-RVM16</t>
+    <t>RCL.PL.STR1</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR2</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR3</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR4</t>
+  </si>
+  <si>
+    <t>RCL.PL.MOP1</t>
+  </si>
+  <si>
+    <t>RCL.PL.MOP2</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR5</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR6</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR7</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR8</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR9</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR10</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR11</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR12</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR13</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR14</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR15</t>
+  </si>
+  <si>
+    <t>The height of the CubeSat system structure shall be 300 mm</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR16</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR17</t>
+  </si>
+  <si>
+    <t>The total CubeSat system volume shall not exceed 6U</t>
+  </si>
+  <si>
+    <t>The total CubeSat system mass shall not exceed 8.0 kg</t>
+  </si>
+  <si>
+    <r>
+      <t>All materials used in the CubeSat system shall have a Total Mass Loss of less than 1.0% (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>List of Low Out-gassing Materials available at outgassing.nasa.gov</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>All materials used in the CubeSat system shall have a Collected Volatile Condensable material of less than 0.1%</t>
+  </si>
+  <si>
+    <t>CubeSat system must be in orbit for at least 6 months</t>
+  </si>
+  <si>
+    <t>CubeSat system must deorbit within 25 years of being launched</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall incorporate a Remove Before Flight pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CubeSat system shall incorporate a deployment switch </t>
+  </si>
+  <si>
+    <t>Center of  gravity of each CubeSat system Jade and Turquoise shall be located within a sphere of 2 cm of the geometric center of said system</t>
+  </si>
+  <si>
+    <t>The CubeSat system coordinate system shall be defined as specified in Figure 1</t>
+  </si>
+  <si>
+    <t>The +Y/-Y Faces of the CubeSat system shall have a length of 100 mm</t>
+  </si>
+  <si>
+    <t>The +X/-X Faces of the CubeSat system shall have a length of 200 mm</t>
+  </si>
+  <si>
+    <t>The payload shall be capable of determining relative distance between Jade and Turquoise</t>
+  </si>
+  <si>
+    <t>CubeSat system shall be capable of recording relative displacement data between Jade and Turquoise</t>
+  </si>
+  <si>
+    <t>Jader and Turquoise separating from one another with a relative velocity no greater than 5 cm/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jade and Turquoise shall achieve a local slew rate of less than 1 deg/s </t>
+  </si>
+  <si>
+    <t>Jade and Turquoise shall record relative displacement between each other</t>
+  </si>
+  <si>
+    <t>Jade and Turquoise shall be able to perform an “escape” maneuver that increases the final relative displacement from the other CubeSat system to at least 100 meters within 1 orbit</t>
+  </si>
+  <si>
+    <t>Jade and Turquoise shall be able to a rendezvous by decreasing the final relative distance from the other CubeSat system to within 50 m for 5 orbits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jade and Turquoise shall be able to stationkeep within a 10-75 m sphere for at least 5 orbits relative to the other CubeSat system </t>
+  </si>
+  <si>
+    <t>RCL.PL.PLD1</t>
+  </si>
+  <si>
+    <t>RCL.PL.PLD2</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR18</t>
+  </si>
+  <si>
+    <t>RCL.PL.PRP1</t>
+  </si>
+  <si>
+    <t>RCL.PL.THM1</t>
+  </si>
+  <si>
+    <t>RCL.PL.PRP2</t>
+  </si>
+  <si>
+    <t>RCL.PL.PRP3</t>
+  </si>
+  <si>
+    <t>RCL.PL.PRP4</t>
+  </si>
+  <si>
+    <t>RCL.PL.TST1</t>
+  </si>
+  <si>
+    <t>RCL.PL.TST2</t>
+  </si>
+  <si>
+    <t>RCL.PL.TST3</t>
+  </si>
+  <si>
+    <t>RCL.PL.TST4</t>
+  </si>
+  <si>
+    <t>RCL.PL.TST5</t>
+  </si>
+  <si>
+    <t>RCL.PLE.MOP1</t>
+  </si>
+  <si>
+    <t>RCL.PLE.MOP2</t>
+  </si>
+  <si>
+    <t>RCL.PLE.MOP3</t>
+  </si>
+  <si>
+    <t>RCL.PLE.MOP4</t>
+  </si>
+  <si>
+    <t>RCL.SS.MOP1</t>
+  </si>
+  <si>
+    <t>RCL.SS.MOP2</t>
+  </si>
+  <si>
+    <t>RCL.SS.MOP3</t>
+  </si>
+  <si>
+    <t>RCL.SK.MOP1</t>
+  </si>
+  <si>
+    <t>RCL.ESC.MOP1</t>
+  </si>
+  <si>
+    <t>RCL.RDZ.MOP1</t>
+  </si>
+  <si>
+    <t>Jade and Turquoise's coordinate system shall be defined as specified in Figure 1</t>
+  </si>
+  <si>
+    <t>RCL.PL.STR19</t>
   </si>
 </sst>
 </file>
@@ -705,7 +724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -890,12 +909,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -971,14 +1012,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1004,21 +1061,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1675,67 +1722,67 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="37">
         <v>41582</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="35"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
@@ -1968,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:IS315"/>
+  <dimension ref="A1:IS318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1989,36 +2036,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:253">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="32" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="41" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:253">
-      <c r="A2" s="37"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="8" t="s">
         <v>55</v>
       </c>
@@ -2031,22 +2078,22 @@
       <c r="H2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="35"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:253">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
     </row>
     <row r="4" spans="1:253" s="10" customFormat="1">
       <c r="A4" s="26" t="s">
@@ -2056,20 +2103,20 @@
         <v>41</v>
       </c>
       <c r="C4" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>60</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>61</v>
       </c>
       <c r="E4" s="26"/>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
       <c r="H4" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I4" s="26"/>
       <c r="J4" s="26" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:253" s="13" customFormat="1">
@@ -2080,20 +2127,20 @@
         <v>41</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="24"/>
       <c r="J5" s="26" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="M5" s="14"/>
       <c r="T5" s="15"/>
@@ -2153,20 +2200,20 @@
         <v>41</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>81</v>
+        <v>123</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="23"/>
       <c r="J6" s="26" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:253" s="10" customFormat="1" ht="30">
@@ -2177,20 +2224,20 @@
         <v>41</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="23"/>
       <c r="J7" s="26" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:253">
@@ -2201,20 +2248,20 @@
         <v>39</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:253" ht="30">
@@ -2225,20 +2272,20 @@
         <v>39</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:253">
@@ -2249,20 +2296,20 @@
         <v>41</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="26" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:253">
@@ -2273,20 +2320,20 @@
         <v>41</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I11" s="23"/>
       <c r="J11" s="26" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:253">
@@ -2297,20 +2344,20 @@
         <v>41</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I12" s="23"/>
       <c r="J12" s="26" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:253" ht="30">
@@ -2321,20 +2368,20 @@
         <v>41</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I13" s="23"/>
       <c r="J13" s="26" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:253" ht="30">
@@ -2345,20 +2392,20 @@
         <v>41</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" s="23"/>
       <c r="J14" s="26" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="V14" s="25"/>
     </row>
@@ -2370,20 +2417,20 @@
         <v>41</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="23"/>
       <c r="J15" s="26" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:253" ht="30">
@@ -2394,23 +2441,23 @@
         <v>41</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>156</v>
+        <v>99</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="16"/>
       <c r="I16" s="24"/>
       <c r="J16" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45">
       <c r="A17" s="16" t="s">
         <v>12</v>
       </c>
@@ -2418,23 +2465,23 @@
         <v>41</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="45" t="s">
-        <v>158</v>
+        <v>129</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>100</v>
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="24"/>
       <c r="J17" s="26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30">
       <c r="A18" s="11" t="s">
         <v>14</v>
       </c>
@@ -2442,47 +2489,47 @@
         <v>41</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="23"/>
       <c r="J18" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
       <c r="A19" s="11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="G19" s="11"/>
-      <c r="H19" s="11" t="s">
-        <v>62</v>
-      </c>
+      <c r="H19" s="11"/>
       <c r="I19" s="23"/>
       <c r="J19" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="30">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30">
       <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2490,71 +2537,71 @@
         <v>41</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="23"/>
       <c r="J20" s="26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30" customHeight="1">
-      <c r="A21" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30">
+      <c r="A21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
-      <c r="A22" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="20" t="s">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="46"/>
+      <c r="J21" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30">
+      <c r="A22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>62</v>
       </c>
+      <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="30">
+      <c r="H22" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" s="30"/>
+      <c r="J22" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -2562,619 +2609,682 @@
         <v>41</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="23"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" s="30"/>
       <c r="J23" s="26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" customHeight="1">
       <c r="A24" s="20" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="20"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30">
+      <c r="A25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30">
+      <c r="A26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20" t="s">
+      <c r="C27" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="30">
-      <c r="A25" s="41" t="s">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="30">
+      <c r="A28" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="42" t="s">
+      <c r="B28" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45">
+      <c r="A29" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45">
+      <c r="A30" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30">
+      <c r="A31" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45">
+      <c r="A32" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30">
+      <c r="A33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="1:11" ht="30">
+      <c r="A34" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="D25" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="45">
-      <c r="A26" s="41" t="s">
+    </row>
+    <row r="35" spans="1:11" ht="30">
+      <c r="A35" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="42" t="s">
+      <c r="B35" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30.75" thickBot="1">
+      <c r="A36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="45">
-      <c r="A27" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="45">
-      <c r="A29" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
-      <c r="A30" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="K30"/>
-    </row>
-    <row r="31" spans="1:11" ht="30">
-      <c r="A31" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30">
-      <c r="A32" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A33" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A34" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="30">
-      <c r="A37" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+    </row>
+    <row r="37" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A37" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
+      <c r="C38" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
       <c r="J38" s="16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-    </row>
-    <row r="40" spans="1:10" ht="30">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="30">
       <c r="A40" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>131</v>
+        <v>24</v>
+      </c>
+      <c r="C40" s="33" t="s">
+        <v>85</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="E40" s="11"/>
-      <c r="F40" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
-      <c r="J40" s="11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="30">
+      <c r="J40" s="16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>155</v>
+        <v>24</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>87</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>154</v>
+        <v>86</v>
       </c>
       <c r="E41" s="11"/>
-      <c r="F41" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
-      <c r="J41" s="11" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="30">
-      <c r="A42" s="16" t="s">
+      <c r="J41" s="16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+    </row>
+    <row r="43" spans="1:11" ht="30">
+      <c r="A43" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="D42" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
-    </row>
-    <row r="44" spans="1:10" ht="45">
+      <c r="D43" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="30">
       <c r="A44" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>138</v>
+        <v>22</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="30">
+      <c r="A45" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+    </row>
+    <row r="47" spans="1:11" ht="30">
+      <c r="A47" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+    </row>
+    <row r="49" spans="1:10" ht="45">
+      <c r="A49" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="40"/>
+      <c r="J50" s="40"/>
+    </row>
+    <row r="51" spans="1:10" ht="45">
+      <c r="A51" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="18" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="34" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
-    </row>
-    <row r="46" spans="1:10" ht="45">
-      <c r="A46" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-    </row>
-    <row r="48" spans="1:10" ht="45">
-      <c r="A48" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3">
-      <c r="C49" s="22"/>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="22"/>
-    </row>
-    <row r="51" spans="3:3">
-      <c r="C51" s="22"/>
-    </row>
-    <row r="52" spans="3:3">
+      <c r="D51" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="C52" s="22"/>
     </row>
-    <row r="53" spans="3:3">
+    <row r="53" spans="1:10">
       <c r="C53" s="22"/>
     </row>
-    <row r="54" spans="3:3">
+    <row r="54" spans="1:10">
       <c r="C54" s="22"/>
     </row>
-    <row r="55" spans="3:3">
+    <row r="55" spans="1:10">
       <c r="C55" s="22"/>
     </row>
-    <row r="56" spans="3:3">
+    <row r="56" spans="1:10">
       <c r="C56" s="22"/>
     </row>
-    <row r="57" spans="3:3">
+    <row r="57" spans="1:10">
       <c r="C57" s="22"/>
     </row>
-    <row r="58" spans="3:3">
+    <row r="58" spans="1:10">
       <c r="C58" s="22"/>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="1:10">
       <c r="C59" s="22"/>
     </row>
-    <row r="60" spans="3:3">
+    <row r="60" spans="1:10">
       <c r="C60" s="22"/>
     </row>
-    <row r="61" spans="3:3">
+    <row r="61" spans="1:10">
       <c r="C61" s="22"/>
     </row>
-    <row r="62" spans="3:3">
+    <row r="62" spans="1:10">
       <c r="C62" s="22"/>
     </row>
-    <row r="63" spans="3:3">
+    <row r="63" spans="1:10">
       <c r="C63" s="22"/>
     </row>
-    <row r="64" spans="3:3">
+    <row r="64" spans="1:10">
       <c r="C64" s="22"/>
     </row>
     <row r="65" spans="3:3">
@@ -3929,6 +4039,15 @@
     </row>
     <row r="315" spans="3:3">
       <c r="C315" s="22"/>
+    </row>
+    <row r="316" spans="3:3">
+      <c r="C316" s="22"/>
+    </row>
+    <row r="317" spans="3:3">
+      <c r="C317" s="22"/>
+    </row>
+    <row r="318" spans="3:3">
+      <c r="C318" s="22"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -3936,13 +4055,13 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="A50:J50"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A48:J48"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -3967,14 +4086,14 @@
   </cols>
   <sheetData>
     <row r="29" spans="4:9">
-      <c r="D29" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
+      <c r="D29" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -4002,14 +4121,14 @@
   </cols>
   <sheetData>
     <row r="40" spans="2:7">
-      <c r="B40" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
+      <c r="B40" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Began creating top level RVM requirements and new task number syntax
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -4,24 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7635" tabRatio="469" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="1" r:id="rId1"/>
     <sheet name="RVM" sheetId="2" r:id="rId2"/>
-    <sheet name="Figure 1-Coordinate System" sheetId="3" r:id="rId3"/>
-    <sheet name="Figure 2- NASA Gevs" sheetId="4" r:id="rId4"/>
+    <sheet name="RVM Rev 1" sheetId="5" r:id="rId3"/>
+    <sheet name="Figure 1-Coordinate System" sheetId="3" r:id="rId4"/>
+    <sheet name="Figure 2- NASA Gevs" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="__Anonymous_Sheet_DB__1">RVM!$D$45</definedName>
   </definedNames>
   <calcPr calcId="125725" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="183">
   <si>
     <t>Document Title</t>
   </si>
@@ -649,12 +649,84 @@
   <si>
     <t>RCL.PL.STR19</t>
   </si>
+  <si>
+    <t>Top Level Requiremetns</t>
+  </si>
+  <si>
+    <t>Mission Stage</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The CubeSat system shall be capable of integrating with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">XXXX </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Deployer</t>
+    </r>
+  </si>
+  <si>
+    <t>As Listed in RCL-DEP Requirements</t>
+  </si>
+  <si>
+    <t>Task Number Syntax</t>
+  </si>
+  <si>
+    <t>PD/I&amp;T</t>
+  </si>
+  <si>
+    <t>RCL-xxx-DEPx</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall be capable of establishing communication between it and a terrestrial source</t>
+  </si>
+  <si>
+    <t>As Listed in RCL-COM Requirements</t>
+  </si>
+  <si>
+    <t>RCL-xxx-COMx</t>
+  </si>
+  <si>
+    <t>Verification Method(s)</t>
+  </si>
+  <si>
+    <t>As Listed in RCL-MOP Requirements</t>
+  </si>
+  <si>
+    <t>RCL-xxx-MOPx</t>
+  </si>
+  <si>
+    <t>As Listed in RCL-ODAR Requirements</t>
+  </si>
+  <si>
+    <t>RCL-xxx-ODARx</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall meet all deorbit/out-gassing requiremetns laid out in Document NPR 8719.14A, NASA Procedural Requirements for Limiting Orbital Debris</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall be capable of operating in a space environment for at least six continuous months</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -703,8 +775,46 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -723,8 +833,20 @@
         <bgColor indexed="62"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -931,12 +1053,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1028,6 +1218,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1061,11 +1257,87 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1722,67 +1994,67 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="39">
         <v>41582</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="35"/>
+      <c r="B8" s="37"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
@@ -2017,8 +2289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IS318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -2036,36 +2308,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:253">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="38" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="43" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:253">
-      <c r="A2" s="43"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="8" t="s">
         <v>55</v>
       </c>
@@ -2078,22 +2350,22 @@
       <c r="H2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="41"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:253">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
     </row>
     <row r="4" spans="1:253" s="10" customFormat="1">
       <c r="A4" s="26" t="s">
@@ -2572,7 +2844,7 @@
       <c r="H21" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="46"/>
+      <c r="I21" s="35"/>
       <c r="J21" s="26" t="s">
         <v>119</v>
       </c>
@@ -2593,7 +2865,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="H22" s="46" t="s">
+      <c r="H22" s="35" t="s">
         <v>61</v>
       </c>
       <c r="I22" s="30"/>
@@ -2617,7 +2889,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
-      <c r="H23" s="46" t="s">
+      <c r="H23" s="35" t="s">
         <v>61</v>
       </c>
       <c r="I23" s="30"/>
@@ -2644,7 +2916,7 @@
         <v>61</v>
       </c>
       <c r="H24" s="20"/>
-      <c r="I24" s="47"/>
+      <c r="I24" s="36"/>
       <c r="J24" s="16" t="s">
         <v>141</v>
       </c>
@@ -2939,18 +3211,18 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="16" t="s">
@@ -3049,18 +3321,18 @@
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42"/>
     </row>
     <row r="43" spans="1:11" ht="30">
       <c r="A43" s="16" t="s">
@@ -3135,18 +3407,18 @@
       </c>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46" s="42"/>
+      <c r="I46" s="42"/>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" spans="1:11" ht="30">
       <c r="A47" s="16" t="s">
@@ -3173,18 +3445,18 @@
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
+      <c r="B48" s="42"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="F48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42"/>
     </row>
     <row r="49" spans="1:10" ht="45">
       <c r="A49" s="16" t="s">
@@ -3211,18 +3483,18 @@
       </c>
     </row>
     <row r="50" spans="1:10">
-      <c r="A50" s="40" t="s">
+      <c r="A50" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="40"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+      <c r="J50" s="42"/>
     </row>
     <row r="51" spans="1:10" ht="45">
       <c r="A51" s="16" t="s">
@@ -4074,6 +4346,444 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="53" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="53"/>
+    <col min="7" max="7" width="19.5703125" style="53" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="53" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.25">
+      <c r="A1" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="14.25">
+      <c r="A2" s="70"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="50"/>
+      <c r="H2" s="52"/>
+    </row>
+    <row r="3" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A3" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+    </row>
+    <row r="4" spans="1:8" ht="30">
+      <c r="A4" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="H4" s="57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30">
+      <c r="A5" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="60"/>
+      <c r="G5" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45">
+      <c r="A6" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="75" t="s">
+        <v>179</v>
+      </c>
+      <c r="H6" s="57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
+      <c r="A7" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="57" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
+      <c r="A8" s="71"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+    </row>
+    <row r="9" spans="1:8" ht="15">
+      <c r="A9" s="71"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+    </row>
+    <row r="10" spans="1:8" ht="15">
+      <c r="A10" s="71"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="57"/>
+    </row>
+    <row r="11" spans="1:8" ht="15">
+      <c r="B11" s="66"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="68"/>
+    </row>
+    <row r="12" spans="1:8" ht="15">
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
+    </row>
+    <row r="13" spans="1:8" ht="15">
+      <c r="B13" s="69"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
+    </row>
+    <row r="14" spans="1:8" ht="15">
+      <c r="B14" s="69"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="68"/>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="B15" s="69"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="B16" s="69"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="68"/>
+    </row>
+    <row r="17" spans="2:8" ht="15">
+      <c r="B17" s="69"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="68"/>
+    </row>
+    <row r="18" spans="2:8" ht="15">
+      <c r="B18" s="69"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="68"/>
+    </row>
+    <row r="19" spans="2:8" ht="15">
+      <c r="B19" s="69"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="68"/>
+    </row>
+    <row r="20" spans="2:8" ht="15">
+      <c r="B20" s="69"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="68"/>
+    </row>
+    <row r="21" spans="2:8" ht="15">
+      <c r="B21" s="69"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="68"/>
+    </row>
+    <row r="22" spans="2:8" ht="15">
+      <c r="B22" s="69"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="68"/>
+    </row>
+    <row r="23" spans="2:8" ht="15">
+      <c r="B23" s="69"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
+    </row>
+    <row r="24" spans="2:8" ht="15">
+      <c r="B24" s="69"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+    </row>
+    <row r="25" spans="2:8" ht="15">
+      <c r="B25" s="69"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+    </row>
+    <row r="26" spans="2:8" ht="15">
+      <c r="B26" s="69"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="68"/>
+    </row>
+    <row r="27" spans="2:8" ht="15">
+      <c r="B27" s="66"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+    </row>
+    <row r="28" spans="2:8" ht="15">
+      <c r="B28" s="69"/>
+      <c r="C28" s="67"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+    </row>
+    <row r="29" spans="2:8" ht="15">
+      <c r="B29" s="69"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+    </row>
+    <row r="30" spans="2:8" ht="15">
+      <c r="B30" s="69"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+    </row>
+    <row r="31" spans="2:8" ht="15">
+      <c r="B31" s="69"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+    </row>
+    <row r="32" spans="2:8" ht="15">
+      <c r="B32" s="69"/>
+      <c r="C32" s="67"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+    </row>
+    <row r="33" spans="2:8" ht="15">
+      <c r="B33" s="69"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+    </row>
+    <row r="34" spans="2:8" ht="15">
+      <c r="B34" s="69"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+    </row>
+    <row r="35" spans="2:8" ht="15">
+      <c r="B35" s="69"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="67"/>
+    </row>
+    <row r="36" spans="2:8" ht="15">
+      <c r="B36" s="69"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D29:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4086,14 +4796,14 @@
   </cols>
   <sheetData>
     <row r="29" spans="4:9">
-      <c r="D29" s="44" t="s">
+      <c r="D29" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -4107,7 +4817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B40:G40"/>
   <sheetViews>
@@ -4121,14 +4831,14 @@
   </cols>
   <sheetData>
     <row r="40" spans="2:7">
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Added requirements for RFP and launch vehicle
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="196">
   <si>
     <t>Document Title</t>
   </si>
@@ -650,10 +650,7 @@
     <t>RCL.PL.STR19</t>
   </si>
   <si>
-    <t>Top Level Requiremetns</t>
-  </si>
-  <si>
-    <t>Mission Stage</t>
+    <t>Top Level Requirements</t>
   </si>
   <si>
     <r>
@@ -720,6 +717,48 @@
   </si>
   <si>
     <t>The CubeSat system shall be capable of operating in a space environment for at least six continuous months</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall be capable of surviving the launch environment described in the NASA GEVS FSFC-STD-7000 Document</t>
+  </si>
+  <si>
+    <t>As Listed in RCL-LAN Requirements</t>
+  </si>
+  <si>
+    <t>RCL-xxx-LANx</t>
+  </si>
+  <si>
+    <t>Verification Mission Stage</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall be capable of meeting each mission requirement specified in the Team Bravo Request for Proposal</t>
+  </si>
+  <si>
+    <t>RCL-xxx-RFPx</t>
+  </si>
+  <si>
+    <t>Deployer Requirements</t>
+  </si>
+  <si>
+    <t>Launch Requirements</t>
+  </si>
+  <si>
+    <t>The CubeSat System shall be subjected to Qualification level random vibration along each of its primary axes as descrbied on Page 2.4-18 of the NPR 8719.14A Document</t>
+  </si>
+  <si>
+    <t>RCL-TST-LAN1</t>
+  </si>
+  <si>
+    <t>Rascal Post-Vibration Testing Assessment Document</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>NOT VERIFIED</t>
+  </si>
+  <si>
+    <t>As Listed in RCL-RFP Requirements</t>
   </si>
 </sst>
 </file>
@@ -1091,17 +1130,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1121,12 +1149,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1257,10 +1298,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1294,18 +1335,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1321,6 +1350,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1338,13 +1370,569 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="44">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -4346,31 +4934,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A10" sqref="A10:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" style="53" customWidth="1"/>
+    <col min="1" max="1" width="25" style="78" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="81" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="53"/>
-    <col min="7" max="7" width="19.5703125" style="53" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" style="53" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="53"/>
+    <col min="7" max="7" width="19.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="80" customWidth="1"/>
+    <col min="9" max="9" width="21" style="53" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.25">
-      <c r="A1" s="70" t="s">
-        <v>167</v>
+    <row r="1" spans="1:9" ht="14.25">
+      <c r="A1" s="67" t="s">
+        <v>185</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
@@ -4378,12 +4967,15 @@
       <c r="G1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="52" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="14.25">
-      <c r="A2" s="70"/>
+      <c r="H1" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.25">
+      <c r="A2" s="67"/>
       <c r="B2" s="50"/>
       <c r="C2" s="54" t="s">
         <v>55</v>
@@ -4398,9 +4990,10 @@
         <v>58</v>
       </c>
       <c r="G2" s="50"/>
-      <c r="H2" s="52"/>
-    </row>
-    <row r="3" spans="1:8" ht="14.25" customHeight="1">
+      <c r="H2" s="50"/>
+      <c r="I2" s="52"/>
+    </row>
+    <row r="3" spans="1:9" ht="14.25" customHeight="1">
       <c r="A3" s="48" t="s">
         <v>166</v>
       </c>
@@ -4411,13 +5004,14 @@
       <c r="F3" s="49"/>
       <c r="G3" s="49"/>
       <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" ht="30">
-      <c r="A4" s="71" t="s">
-        <v>171</v>
+      <c r="I3" s="49"/>
+    </row>
+    <row r="4" spans="1:9" ht="30">
+      <c r="A4" s="68" t="s">
+        <v>170</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C4" s="57"/>
       <c r="D4" s="57" t="s">
@@ -4429,354 +5023,522 @@
       <c r="F4" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="72" t="s">
-        <v>169</v>
-      </c>
-      <c r="H4" s="57" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30">
-      <c r="A5" s="71" t="s">
+      <c r="G4" s="69" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="I4" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="B5" s="59" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="45">
+      <c r="A5" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="74" t="s">
-        <v>177</v>
-      </c>
-      <c r="H5" s="57" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="71" t="s">
-        <v>14</v>
+      <c r="C5" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="69" t="s">
+        <v>183</v>
+      </c>
+      <c r="H5" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="I5" s="57" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="68" t="s">
+        <v>170</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="75" t="s">
+      <c r="C6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="58"/>
+      <c r="G6" s="71" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="I6" s="74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45">
+      <c r="A7" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="H7" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="I7" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="H6" s="57" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30">
-      <c r="A7" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="73" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="30">
+      <c r="A8" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="58"/>
+      <c r="G8" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="C7" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="74" t="s">
+      <c r="H8" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="I8" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="H7" s="57" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15">
-      <c r="A8" s="71"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-    </row>
-    <row r="9" spans="1:8" ht="15">
-      <c r="A9" s="71"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-    </row>
-    <row r="10" spans="1:8" ht="15">
-      <c r="A10" s="71"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="57"/>
-    </row>
-    <row r="11" spans="1:8" ht="15">
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
-    </row>
-    <row r="12" spans="1:8" ht="15">
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
-    </row>
-    <row r="13" spans="1:8" ht="15">
-      <c r="B13" s="69"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
-    </row>
-    <row r="14" spans="1:8" ht="15">
-      <c r="B14" s="69"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
-    </row>
-    <row r="15" spans="1:8" ht="15">
-      <c r="B15" s="69"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
-    </row>
-    <row r="16" spans="1:8" ht="15">
-      <c r="B16" s="69"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
-    </row>
-    <row r="17" spans="2:8" ht="15">
-      <c r="B17" s="69"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
-    </row>
-    <row r="18" spans="2:8" ht="15">
-      <c r="B18" s="69"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="68"/>
-    </row>
-    <row r="19" spans="2:8" ht="15">
-      <c r="B19" s="69"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
-    </row>
-    <row r="20" spans="2:8" ht="15">
-      <c r="B20" s="69"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="68"/>
-    </row>
-    <row r="21" spans="2:8" ht="15">
-      <c r="B21" s="69"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="68"/>
-    </row>
-    <row r="22" spans="2:8" ht="15">
-      <c r="B22" s="69"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="68"/>
-    </row>
-    <row r="23" spans="2:8" ht="15">
-      <c r="B23" s="69"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="68"/>
-    </row>
-    <row r="24" spans="2:8" ht="15">
-      <c r="B24" s="69"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-    </row>
-    <row r="25" spans="2:8" ht="15">
-      <c r="B25" s="69"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-    </row>
-    <row r="26" spans="2:8" ht="15">
-      <c r="B26" s="69"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="68"/>
-    </row>
-    <row r="27" spans="2:8" ht="15">
-      <c r="B27" s="66"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-    </row>
-    <row r="28" spans="2:8" ht="15">
-      <c r="B28" s="69"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
-      <c r="H28" s="67"/>
-    </row>
-    <row r="29" spans="2:8" ht="15">
-      <c r="B29" s="69"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-    </row>
-    <row r="30" spans="2:8" ht="15">
-      <c r="B30" s="69"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-    </row>
-    <row r="31" spans="2:8" ht="15">
-      <c r="B31" s="69"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-    </row>
-    <row r="32" spans="2:8" ht="15">
-      <c r="B32" s="69"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-    </row>
-    <row r="33" spans="2:8" ht="15">
-      <c r="B33" s="69"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
-      <c r="H33" s="67"/>
-    </row>
-    <row r="34" spans="2:8" ht="15">
-      <c r="B34" s="69"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-    </row>
-    <row r="35" spans="2:8" ht="15">
-      <c r="B35" s="69"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-    </row>
-    <row r="36" spans="2:8" ht="15">
-      <c r="B36" s="69"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
+    </row>
+    <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="75" t="s">
+        <v>195</v>
+      </c>
+      <c r="H9" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="I9" s="60" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+    </row>
+    <row r="11" spans="1:9" ht="15">
+      <c r="A11" s="68"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I11" s="57"/>
+    </row>
+    <row r="12" spans="1:9" ht="15">
+      <c r="A12" s="68"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I12" s="57"/>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="A13" s="68"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" s="57"/>
+    </row>
+    <row r="14" spans="1:9" ht="15">
+      <c r="A14" s="68"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" ht="15">
+      <c r="A15" s="68"/>
+      <c r="B15" s="76"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I15" s="57"/>
+    </row>
+    <row r="16" spans="1:9" ht="15">
+      <c r="A16" s="68"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I16" s="57"/>
+    </row>
+    <row r="17" spans="1:9" ht="15">
+      <c r="A17" s="68"/>
+      <c r="B17" s="76"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I17" s="57"/>
+    </row>
+    <row r="18" spans="1:9" ht="15">
+      <c r="A18" s="68"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" s="57"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="48" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="49"/>
+      <c r="C19" s="49"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+    </row>
+    <row r="20" spans="1:9" ht="60">
+      <c r="A20" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>190</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="79" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20" s="57" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="A21" s="68"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I21" s="57"/>
+    </row>
+    <row r="22" spans="1:9" ht="15">
+      <c r="A22" s="68"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I22" s="57"/>
+    </row>
+    <row r="23" spans="1:9" ht="15">
+      <c r="A23" s="68"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I23" s="57"/>
+    </row>
+    <row r="24" spans="1:9" ht="15">
+      <c r="A24" s="68"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79" t="s">
+        <v>194</v>
+      </c>
+      <c r="I24" s="57"/>
+    </row>
+    <row r="25" spans="1:9" ht="15">
+      <c r="B25" s="65"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="63"/>
+    </row>
+    <row r="26" spans="1:9" ht="15">
+      <c r="B26" s="65"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="63"/>
+    </row>
+    <row r="27" spans="1:9" ht="15">
+      <c r="B27" s="65"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="64"/>
+    </row>
+    <row r="28" spans="1:9" ht="15">
+      <c r="B28" s="62"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
+      <c r="I28" s="63"/>
+    </row>
+    <row r="29" spans="1:9" ht="15">
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="63"/>
+    </row>
+    <row r="30" spans="1:9" ht="15">
+      <c r="B30" s="65"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="63"/>
+    </row>
+    <row r="31" spans="1:9" ht="15">
+      <c r="B31" s="65"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
+      <c r="I31" s="63"/>
+    </row>
+    <row r="32" spans="1:9" ht="15">
+      <c r="B32" s="65"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="63"/>
+    </row>
+    <row r="33" spans="2:9" ht="15">
+      <c r="B33" s="65"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="63"/>
+    </row>
+    <row r="34" spans="2:9" ht="15">
+      <c r="B34" s="65"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="63"/>
+    </row>
+    <row r="35" spans="2:9" ht="15">
+      <c r="B35" s="65"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="63"/>
+    </row>
+    <row r="36" spans="2:9" ht="15">
+      <c r="B36" s="65"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="63"/>
+    </row>
+    <row r="37" spans="2:9" ht="15">
+      <c r="B37" s="65"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A19:I19"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:G2"/>
   </mergeCells>
+  <conditionalFormatting sqref="H4:H9">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+      <formula>"VERIFIED"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11:H18">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>"NOT VERIFIED"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",H11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20:H1048576">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"NOT VERIFIED"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",H20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added two mission operation requirements
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="213">
   <si>
     <t>Document Title</t>
   </si>
@@ -759,6 +759,57 @@
   </si>
   <si>
     <t>As Listed in RCL-RFP Requirements</t>
+  </si>
+  <si>
+    <t>Mission Operations Requirements</t>
+  </si>
+  <si>
+    <t>ODAR Requirements</t>
+  </si>
+  <si>
+    <t>Communication Requirements</t>
+  </si>
+  <si>
+    <t>RFP Requirements</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall be capable of deorbiting within 25 years of its launch date</t>
+  </si>
+  <si>
+    <t>RCL-PD-ODAR1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rascal Orbital Analysis Document </t>
+  </si>
+  <si>
+    <t>All materials used in the CubeSat system shall have a Total Mass Loss of less than 1.0% (List of Low Out-gassing Materials available at outgassing.nasa.gov)</t>
+  </si>
+  <si>
+    <t>Rascal System Materials List</t>
+  </si>
+  <si>
+    <t>RCL-PD-ODAR2</t>
+  </si>
+  <si>
+    <t>RCL-PD-ODAR3</t>
+  </si>
+  <si>
+    <t>The CubeSat system shall have a power system capable of continuous operations of at least 6 months</t>
+  </si>
+  <si>
+    <t>RCL-PD-MOP1</t>
+  </si>
+  <si>
+    <t>Rascal Power Budget Document</t>
+  </si>
+  <si>
+    <t>All components and electrical systems used in the CubeSat system must be capable of withstanding the radition environment associated with Earth-Orbit for at least 6 months</t>
+  </si>
+  <si>
+    <t>RCL-PD-MOP2</t>
+  </si>
+  <si>
+    <t>Rascal Radiation Mitigation Document</t>
   </si>
 </sst>
 </file>
@@ -1167,7 +1218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1320,6 +1371,7 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1338,21 +1390,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,13 +1434,19 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="43">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1540,11 +1583,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1552,11 +1595,11 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1905,18 +1948,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2877,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IS318"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -4934,25 +4965,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25" style="78" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" style="81" customWidth="1"/>
+    <col min="1" max="1" width="25" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="77" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="53"/>
-    <col min="7" max="7" width="19.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="80" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="76" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="76" customWidth="1"/>
     <col min="9" max="9" width="21" style="53" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="63" t="s">
         <v>185</v>
       </c>
       <c r="B1" s="50" t="s">
@@ -4975,7 +5006,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
-      <c r="A2" s="67"/>
+      <c r="A2" s="63"/>
       <c r="B2" s="50"/>
       <c r="C2" s="54" t="s">
         <v>55</v>
@@ -5007,158 +5038,158 @@
       <c r="I3" s="49"/>
     </row>
     <row r="4" spans="1:9" ht="30">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="69" t="s">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="H4" s="69" t="s">
+      <c r="H4" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="58" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="C5" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="69" t="s">
+      <c r="C5" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="65" t="s">
         <v>183</v>
       </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="58" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="71" t="s">
+      <c r="C6" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="59"/>
+      <c r="G6" s="67" t="s">
         <v>176</v>
       </c>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="I6" s="74" t="s">
+      <c r="I6" s="70" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="60" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="72" t="s">
+      <c r="C7" s="61"/>
+      <c r="D7" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="68" t="s">
         <v>178</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="58" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="66" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="71" t="s">
+      <c r="C8" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="59"/>
+      <c r="G8" s="67" t="s">
         <v>173</v>
       </c>
-      <c r="H8" s="69" t="s">
+      <c r="H8" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="58" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="C9" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="60" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="75" t="s">
+      <c r="C9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="H9" s="69" t="s">
+      <c r="H9" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="I9" s="60" t="s">
+      <c r="I9" s="61" t="s">
         <v>187</v>
       </c>
     </row>
@@ -5176,108 +5207,108 @@
       <c r="I10" s="49"/>
     </row>
     <row r="11" spans="1:9" ht="15">
-      <c r="A11" s="68"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61" t="s">
+      <c r="A11" s="64"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I11" s="57"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="1:9" ht="15">
-      <c r="A12" s="68"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61" t="s">
+      <c r="A12" s="64"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I12" s="57"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="15">
-      <c r="A13" s="68"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61" t="s">
+      <c r="A13" s="64"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I13" s="57"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="1:9" ht="15">
-      <c r="A14" s="68"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61" t="s">
+      <c r="A14" s="64"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I14" s="57"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="1:9" ht="15">
-      <c r="A15" s="68"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61" t="s">
+      <c r="A15" s="64"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I15" s="57"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="1:9" ht="15">
-      <c r="A16" s="68"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61" t="s">
+      <c r="A16" s="64"/>
+      <c r="B16" s="72"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I16" s="57"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="1:9" ht="15">
-      <c r="A17" s="68"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61" t="s">
+      <c r="A17" s="64"/>
+      <c r="B17" s="72"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I17" s="57"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="1:9" ht="15">
-      <c r="A18" s="68"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61" t="s">
+      <c r="A18" s="64"/>
+      <c r="B18" s="72"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="I18" s="57"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="48" t="s">
@@ -5293,212 +5324,532 @@
       <c r="I19" s="49"/>
     </row>
     <row r="20" spans="1:9" ht="60">
-      <c r="A20" s="68" t="s">
+      <c r="A20" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="76" t="s">
+      <c r="B20" s="72" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="79" t="s">
+      <c r="C20" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="75" t="s">
         <v>192</v>
       </c>
-      <c r="H20" s="79" t="s">
+      <c r="H20" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="I20" s="57" t="s">
+      <c r="I20" s="58" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15">
-      <c r="A21" s="68"/>
-      <c r="B21" s="76"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79" t="s">
+      <c r="A21" s="64"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="I21" s="57"/>
+      <c r="I21" s="58"/>
     </row>
     <row r="22" spans="1:9" ht="15">
-      <c r="A22" s="68"/>
-      <c r="B22" s="76"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79" t="s">
+      <c r="A22" s="64"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="I22" s="57"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:9" ht="15">
-      <c r="A23" s="68"/>
-      <c r="B23" s="76"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79" t="s">
+      <c r="A23" s="64"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="I23" s="57"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="1:9" ht="15">
-      <c r="A24" s="68"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79" t="s">
+      <c r="A24" s="64"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75" t="s">
         <v>194</v>
       </c>
-      <c r="I24" s="57"/>
-    </row>
-    <row r="25" spans="1:9" ht="15">
-      <c r="B25" s="65"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="63"/>
-    </row>
-    <row r="26" spans="1:9" ht="15">
-      <c r="B26" s="65"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="63"/>
-    </row>
-    <row r="27" spans="1:9" ht="15">
-      <c r="B27" s="65"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="64"/>
+      <c r="I24" s="58"/>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" s="49"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+    </row>
+    <row r="26" spans="1:9" ht="30">
+      <c r="A26" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="62"/>
+      <c r="G26" s="75" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="I26" s="62" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45">
+      <c r="A27" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="72" t="s">
+        <v>210</v>
+      </c>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="75" t="s">
+        <v>212</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="I27" s="62" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="15">
-      <c r="B28" s="62"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="63"/>
+      <c r="A28" s="64"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="62"/>
     </row>
     <row r="29" spans="1:9" ht="15">
-      <c r="B29" s="65"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="63"/>
+      <c r="A29" s="64"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="62"/>
     </row>
     <row r="30" spans="1:9" ht="15">
-      <c r="B30" s="65"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="63"/>
-    </row>
-    <row r="31" spans="1:9" ht="15">
-      <c r="B31" s="65"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="63"/>
-    </row>
-    <row r="32" spans="1:9" ht="15">
-      <c r="B32" s="65"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="63"/>
-    </row>
-    <row r="33" spans="2:9" ht="15">
-      <c r="B33" s="65"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="63"/>
-    </row>
-    <row r="34" spans="2:9" ht="15">
-      <c r="B34" s="65"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="66"/>
-      <c r="I34" s="63"/>
-    </row>
-    <row r="35" spans="2:9" ht="15">
-      <c r="B35" s="65"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="63"/>
-    </row>
-    <row r="36" spans="2:9" ht="15">
-      <c r="B36" s="65"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="63"/>
-    </row>
-    <row r="37" spans="2:9" ht="15">
-      <c r="B37" s="65"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="63"/>
+      <c r="A30" s="64"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="62"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+    </row>
+    <row r="32" spans="1:9" ht="30">
+      <c r="A32" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="72" t="s">
+        <v>200</v>
+      </c>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="75" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="I32" s="62" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45">
+      <c r="A33" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="H33" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="I33" s="62" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30">
+      <c r="A34" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="75" t="s">
+        <v>204</v>
+      </c>
+      <c r="H34" s="75" t="s">
+        <v>194</v>
+      </c>
+      <c r="I34" s="62" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="64"/>
+      <c r="B36" s="78"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="56"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="64"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="56"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="64"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="56"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="64"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="56"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="56"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="64"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="56"/>
+      <c r="G40" s="79"/>
+      <c r="H40" s="79"/>
+      <c r="I40" s="56"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="64"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="56"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="56"/>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="64"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="79"/>
+      <c r="I42" s="56"/>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="64"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="56"/>
+      <c r="G43" s="79"/>
+      <c r="H43" s="79"/>
+      <c r="I43" s="56"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="64"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="79"/>
+      <c r="I45" s="56"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="64"/>
+      <c r="B46" s="78"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="79"/>
+      <c r="I46" s="56"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="64"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="79"/>
+      <c r="H47" s="79"/>
+      <c r="I47" s="56"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="64"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="56"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="64"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="79"/>
+      <c r="H49" s="79"/>
+      <c r="I49" s="56"/>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="64"/>
+      <c r="B50" s="78"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="79"/>
+      <c r="H50" s="79"/>
+      <c r="I50" s="56"/>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="64"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="56"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="64"/>
+      <c r="B52" s="78"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="56"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="64"/>
+      <c r="B53" s="78"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="79"/>
+      <c r="I53" s="56"/>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="64"/>
+      <c r="B54" s="78"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="56"/>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="64"/>
+      <c r="B55" s="78"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="79"/>
+      <c r="H55" s="79"/>
+      <c r="I55" s="56"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="64"/>
+      <c r="B56" s="78"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="56"/>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="64"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="56"/>
+      <c r="G57" s="79"/>
+      <c r="H57" s="79"/>
+      <c r="I57" s="56"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="64"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="56"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="A25:I25"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A44:I44"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A10:I10"/>
@@ -5510,33 +5861,33 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H4)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"VERIFIED"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="NOT VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H4)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32:H34 H11:H18 H20:H24 H26:H30">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",H11)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"NOT VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H18">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+  <conditionalFormatting sqref="H36:H43 H45:H1048576">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H36)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",H36)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"NOT VERIFIED"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("VERIFIED",H11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="NOT VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H1048576">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"NOT VERIFIED"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("VERIFIED",H20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NOT VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added launch integration requirement
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="216">
   <si>
     <t>Document Title</t>
   </si>
@@ -680,9 +680,6 @@
     <t>As Listed in RCL-DEP Requirements</t>
   </si>
   <si>
-    <t>Task Number Syntax</t>
-  </si>
-  <si>
     <t>PD/I&amp;T</t>
   </si>
   <si>
@@ -810,6 +807,18 @@
   </si>
   <si>
     <t>Rascal Radiation Mitigation Document</t>
+  </si>
+  <si>
+    <t>All components and electrical systems used in the CubeSat system must be capable of withstanding the thermal enviroment associated with Earth-Orbit for at least 6 months</t>
+  </si>
+  <si>
+    <t>Rascal Thermal Analysis Document</t>
+  </si>
+  <si>
+    <t>RCL-PD-MOP3</t>
+  </si>
+  <si>
+    <t>Task Number Taxonomy</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1455,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="21">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1696,270 +1705,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4967,8 +4712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4978,19 +4723,19 @@
     <col min="3" max="6" width="9.140625" style="53"/>
     <col min="7" max="7" width="19.5703125" style="76" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" style="76" customWidth="1"/>
-    <col min="9" max="9" width="21" style="53" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="53" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.25">
       <c r="A1" s="63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
@@ -4999,10 +4744,10 @@
         <v>53</v>
       </c>
       <c r="H1" s="50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I1" s="52" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.25">
@@ -5039,7 +4784,7 @@
     </row>
     <row r="4" spans="1:9" ht="30">
       <c r="A4" s="64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="57" t="s">
         <v>167</v>
@@ -5058,10 +4803,10 @@
         <v>168</v>
       </c>
       <c r="H4" s="65" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I4" s="58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45">
@@ -5069,7 +4814,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C5" s="58" t="s">
         <v>61</v>
@@ -5078,21 +4823,21 @@
       <c r="E5" s="58"/>
       <c r="F5" s="58"/>
       <c r="G5" s="65" t="s">
+        <v>182</v>
+      </c>
+      <c r="H5" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="I5" s="58" t="s">
         <v>183</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30">
       <c r="A6" s="64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" s="59" t="s">
         <v>61</v>
@@ -5105,13 +4850,13 @@
       </c>
       <c r="F6" s="59"/>
       <c r="G6" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" s="70" t="s">
         <v>176</v>
-      </c>
-      <c r="H6" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45">
@@ -5119,7 +4864,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="61" t="s">
@@ -5128,21 +4873,21 @@
       <c r="E7" s="61"/>
       <c r="F7" s="61"/>
       <c r="G7" s="68" t="s">
+        <v>177</v>
+      </c>
+      <c r="H7" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="I7" s="58" t="s">
         <v>178</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
       <c r="A8" s="64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C8" s="59" t="s">
         <v>61</v>
@@ -5155,47 +4900,47 @@
       </c>
       <c r="F8" s="59"/>
       <c r="G8" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="I8" s="58" t="s">
         <v>173</v>
-      </c>
-      <c r="H8" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
       <c r="A9" s="64" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>194</v>
+      </c>
+      <c r="H9" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9" s="61" t="s">
         <v>186</v>
-      </c>
-      <c r="C9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>195</v>
-      </c>
-      <c r="H9" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="I9" s="61" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
@@ -5215,7 +4960,7 @@
       <c r="F11" s="62"/>
       <c r="G11" s="62"/>
       <c r="H11" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I11" s="58"/>
     </row>
@@ -5228,7 +4973,7 @@
       <c r="F12" s="62"/>
       <c r="G12" s="62"/>
       <c r="H12" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I12" s="58"/>
     </row>
@@ -5241,7 +4986,7 @@
       <c r="F13" s="62"/>
       <c r="G13" s="62"/>
       <c r="H13" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I13" s="58"/>
     </row>
@@ -5254,7 +4999,7 @@
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
       <c r="H14" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I14" s="58"/>
     </row>
@@ -5267,7 +5012,7 @@
       <c r="F15" s="62"/>
       <c r="G15" s="62"/>
       <c r="H15" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I15" s="58"/>
     </row>
@@ -5280,7 +5025,7 @@
       <c r="F16" s="62"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I16" s="58"/>
     </row>
@@ -5293,7 +5038,7 @@
       <c r="F17" s="62"/>
       <c r="G17" s="62"/>
       <c r="H17" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I17" s="58"/>
     </row>
@@ -5306,13 +5051,13 @@
       <c r="F18" s="62"/>
       <c r="G18" s="62"/>
       <c r="H18" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I18" s="58"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
@@ -5328,7 +5073,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="72" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C20" s="62" t="s">
         <v>61</v>
@@ -5337,13 +5082,13 @@
       <c r="E20" s="62"/>
       <c r="F20" s="62"/>
       <c r="G20" s="75" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H20" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I20" s="58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15">
@@ -5355,7 +5100,7 @@
       <c r="F21" s="62"/>
       <c r="G21" s="75"/>
       <c r="H21" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I21" s="58"/>
     </row>
@@ -5368,7 +5113,7 @@
       <c r="F22" s="62"/>
       <c r="G22" s="75"/>
       <c r="H22" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I22" s="58"/>
     </row>
@@ -5381,7 +5126,7 @@
       <c r="F23" s="62"/>
       <c r="G23" s="75"/>
       <c r="H23" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I23" s="58"/>
     </row>
@@ -5394,13 +5139,13 @@
       <c r="F24" s="62"/>
       <c r="G24" s="75"/>
       <c r="H24" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I24" s="58"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
@@ -5416,7 +5161,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C26" s="62" t="s">
         <v>61</v>
@@ -5429,13 +5174,13 @@
       </c>
       <c r="F26" s="62"/>
       <c r="G26" s="75" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H26" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I26" s="62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45">
@@ -5443,7 +5188,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C27" s="62"/>
       <c r="D27" s="62" t="s">
@@ -5452,25 +5197,39 @@
       <c r="E27" s="62"/>
       <c r="F27" s="62"/>
       <c r="G27" s="75" t="s">
+        <v>211</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>193</v>
+      </c>
+      <c r="I27" s="62" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="45">
+      <c r="A28" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="72" t="s">
         <v>212</v>
       </c>
-      <c r="H27" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="I27" s="62" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="15">
-      <c r="A28" s="64"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
+      <c r="C28" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="62" t="s">
+        <v>61</v>
+      </c>
       <c r="E28" s="62"/>
       <c r="F28" s="62"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="62"/>
+      <c r="G28" s="75" t="s">
+        <v>213</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>193</v>
+      </c>
+      <c r="I28" s="62" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="15">
       <c r="A29" s="64"/>
@@ -5496,7 +5255,7 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31" s="49"/>
       <c r="C31" s="49"/>
@@ -5512,7 +5271,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C32" s="62"/>
       <c r="D32" s="62" t="s">
@@ -5521,13 +5280,13 @@
       <c r="E32" s="62"/>
       <c r="F32" s="62"/>
       <c r="G32" s="75" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H32" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I32" s="62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="45">
@@ -5535,7 +5294,7 @@
         <v>14</v>
       </c>
       <c r="B33" s="72" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C33" s="62"/>
       <c r="D33" s="62" t="s">
@@ -5544,13 +5303,13 @@
       <c r="E33" s="62"/>
       <c r="F33" s="62"/>
       <c r="G33" s="75" t="s">
+        <v>203</v>
+      </c>
+      <c r="H33" s="75" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="62" t="s">
         <v>204</v>
-      </c>
-      <c r="H33" s="75" t="s">
-        <v>194</v>
-      </c>
-      <c r="I33" s="62" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30">
@@ -5567,18 +5326,18 @@
       <c r="E34" s="62"/>
       <c r="F34" s="62"/>
       <c r="G34" s="75" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H34" s="75" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I34" s="62" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="49"/>
@@ -5679,7 +5438,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B44" s="49"/>
       <c r="C44" s="49"/>

</xml_diff>

<commit_message>
Changed top level requirements to reflect RFP requirements
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="196">
   <si>
     <t>Document Title</t>
   </si>
@@ -653,111 +653,24 @@
     <t>Top Level Requirements</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">The CubeSat system shall be capable of integrating with the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">XXXX </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Deployer</t>
-    </r>
-  </si>
-  <si>
-    <t>As Listed in RCL-DEP Requirements</t>
-  </si>
-  <si>
     <t>PD/I&amp;T</t>
   </si>
   <si>
-    <t>RCL-xxx-DEPx</t>
-  </si>
-  <si>
-    <t>The CubeSat system shall be capable of establishing communication between it and a terrestrial source</t>
-  </si>
-  <si>
-    <t>As Listed in RCL-COM Requirements</t>
-  </si>
-  <si>
-    <t>RCL-xxx-COMx</t>
-  </si>
-  <si>
     <t>Verification Method(s)</t>
   </si>
   <si>
-    <t>As Listed in RCL-MOP Requirements</t>
-  </si>
-  <si>
-    <t>RCL-xxx-MOPx</t>
-  </si>
-  <si>
-    <t>As Listed in RCL-ODAR Requirements</t>
-  </si>
-  <si>
-    <t>RCL-xxx-ODARx</t>
-  </si>
-  <si>
-    <t>The CubeSat system shall meet all deorbit/out-gassing requiremetns laid out in Document NPR 8719.14A, NASA Procedural Requirements for Limiting Orbital Debris</t>
-  </si>
-  <si>
-    <t>The CubeSat system shall be capable of operating in a space environment for at least six continuous months</t>
-  </si>
-  <si>
-    <t>The CubeSat system shall be capable of surviving the launch environment described in the NASA GEVS FSFC-STD-7000 Document</t>
-  </si>
-  <si>
-    <t>As Listed in RCL-LAN Requirements</t>
-  </si>
-  <si>
-    <t>RCL-xxx-LANx</t>
-  </si>
-  <si>
     <t>Verification Mission Stage</t>
   </si>
   <si>
-    <t>The CubeSat system shall be capable of meeting each mission requirement specified in the Team Bravo Request for Proposal</t>
-  </si>
-  <si>
-    <t>RCL-xxx-RFPx</t>
-  </si>
-  <si>
-    <t>Deployer Requirements</t>
-  </si>
-  <si>
     <t>Launch Requirements</t>
   </si>
   <si>
-    <t>The CubeSat System shall be subjected to Qualification level random vibration along each of its primary axes as descrbied on Page 2.4-18 of the NPR 8719.14A Document</t>
-  </si>
-  <si>
-    <t>RCL-TST-LAN1</t>
-  </si>
-  <si>
-    <t>Rascal Post-Vibration Testing Assessment Document</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>NOT VERIFIED</t>
   </si>
   <si>
-    <t>As Listed in RCL-RFP Requirements</t>
-  </si>
-  <si>
     <t>Mission Operations Requirements</t>
   </si>
   <si>
@@ -770,62 +683,68 @@
     <t>RFP Requirements</t>
   </si>
   <si>
-    <t>The CubeSat system shall be capable of deorbiting within 25 years of its launch date</t>
-  </si>
-  <si>
-    <t>RCL-PD-ODAR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rascal Orbital Analysis Document </t>
-  </si>
-  <si>
-    <t>All materials used in the CubeSat system shall have a Total Mass Loss of less than 1.0% (List of Low Out-gassing Materials available at outgassing.nasa.gov)</t>
-  </si>
-  <si>
-    <t>Rascal System Materials List</t>
-  </si>
-  <si>
-    <t>RCL-PD-ODAR2</t>
-  </si>
-  <si>
-    <t>RCL-PD-ODAR3</t>
-  </si>
-  <si>
-    <t>The CubeSat system shall have a power system capable of continuous operations of at least 6 months</t>
-  </si>
-  <si>
-    <t>RCL-PD-MOP1</t>
-  </si>
-  <si>
-    <t>Rascal Power Budget Document</t>
-  </si>
-  <si>
-    <t>All components and electrical systems used in the CubeSat system must be capable of withstanding the radition environment associated with Earth-Orbit for at least 6 months</t>
-  </si>
-  <si>
-    <t>RCL-PD-MOP2</t>
-  </si>
-  <si>
-    <t>Rascal Radiation Mitigation Document</t>
-  </si>
-  <si>
-    <t>All components and electrical systems used in the CubeSat system must be capable of withstanding the thermal enviroment associated with Earth-Orbit for at least 6 months</t>
-  </si>
-  <si>
-    <t>Rascal Thermal Analysis Document</t>
-  </si>
-  <si>
-    <t>RCL-PD-MOP3</t>
-  </si>
-  <si>
     <t>Task Number Taxonomy</t>
+  </si>
+  <si>
+    <t>The spacecraft must be capable of demonstrating station keeping within a 50 meter sphere of a resident space object for at least 5 orbits</t>
+  </si>
+  <si>
+    <t>The spacecraft must be capable of demonstrating an "Escape" maneuver by intentionally increasting the relative distance between it and a relative space object to at lest 100 meters within one orbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD </t>
+  </si>
+  <si>
+    <t>The spacecraft shall be capable of demonstrating rendezvous with by intentionally reducing the deistance between it and a resident space object to at most 50 meters for at least 5 orbits</t>
+  </si>
+  <si>
+    <t>A method of verifying the successful completion of each mission requirement shall be incorperated into the spacecraft design and mission operations procedures</t>
+  </si>
+  <si>
+    <t>RCL-RFP1-x</t>
+  </si>
+  <si>
+    <t>RCL-RFP2-x</t>
+  </si>
+  <si>
+    <t>RCL-RFP3-x</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-x</t>
+  </si>
+  <si>
+    <t>RCL-MOP2-x</t>
+  </si>
+  <si>
+    <t>Rationale</t>
+  </si>
+  <si>
+    <t>RFP Requirement</t>
+  </si>
+  <si>
+    <t>Mission Operations Requirement</t>
+  </si>
+  <si>
+    <t>The sapcecraft mission shall be executed within 6 months of spacecraft launch</t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize the CubeSat standard architecture</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Architecture Requirements</t>
+  </si>
+  <si>
+    <t>RCL-ARC1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -890,13 +809,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color indexed="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -945,7 +857,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1155,30 +1067,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
@@ -1227,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1358,96 +1246,95 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1455,199 +1342,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2344,7 +2039,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4710,48 +4405,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="25" style="74" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.28515625" style="77" customWidth="1"/>
+    <col min="1" max="1" width="25" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.28515625" style="70" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="53"/>
-    <col min="7" max="7" width="19.5703125" style="76" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="76" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="53"/>
+    <col min="7" max="7" width="18.5703125" style="53" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="69" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="69" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="53" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25">
-      <c r="A1" s="63" t="s">
-        <v>184</v>
+    <row r="1" spans="1:10" ht="14.25">
+      <c r="A1" s="60" t="s">
+        <v>169</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="50" t="s">
-        <v>192</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.25">
-      <c r="A2" s="63"/>
+      <c r="I1" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.25">
+      <c r="A2" s="60"/>
       <c r="B2" s="50"/>
       <c r="C2" s="54" t="s">
         <v>55</v>
@@ -4767,9 +4466,10 @@
       </c>
       <c r="G2" s="50"/>
       <c r="H2" s="50"/>
-      <c r="I2" s="52"/>
-    </row>
-    <row r="3" spans="1:9" ht="14.25" customHeight="1">
+      <c r="I2" s="50"/>
+      <c r="J2" s="52"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.25" customHeight="1">
       <c r="A3" s="48" t="s">
         <v>166</v>
       </c>
@@ -4781,871 +4481,791 @@
       <c r="G3" s="49"/>
       <c r="H3" s="49"/>
       <c r="I3" s="49"/>
-    </row>
-    <row r="4" spans="1:9" ht="30">
-      <c r="A4" s="64" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="57" t="s">
+      <c r="J3" s="49"/>
+    </row>
+    <row r="4" spans="1:10" ht="45">
+      <c r="A4" s="72" t="s">
         <v>167</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="H4" s="65" t="s">
+      <c r="B4" s="76" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="H4" s="77"/>
+      <c r="I4" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J4" s="72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45">
+      <c r="A5" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="H5" s="77"/>
+      <c r="I5" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J5" s="72" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45">
+      <c r="A6" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="H6" s="77"/>
+      <c r="I6" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J6" s="72" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45">
+      <c r="A7" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="H7" s="63"/>
+      <c r="I7" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="J7" s="64" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30">
+      <c r="A8" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="H8" s="63"/>
+      <c r="I8" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" s="64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+    </row>
+    <row r="10" spans="1:10" ht="15">
+      <c r="A10" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="H10" s="59"/>
+      <c r="I10" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" s="56" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15">
+      <c r="A11" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" s="56"/>
+    </row>
+    <row r="12" spans="1:10" ht="15">
+      <c r="A12" s="72"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="56"/>
+    </row>
+    <row r="13" spans="1:10" ht="15">
+      <c r="A13" s="72"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="56"/>
+    </row>
+    <row r="14" spans="1:10" ht="15">
+      <c r="A14" s="72"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="56"/>
+    </row>
+    <row r="15" spans="1:10" ht="15">
+      <c r="A15" s="72"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J15" s="56"/>
+    </row>
+    <row r="16" spans="1:10" ht="15">
+      <c r="A16" s="72"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J16" s="56"/>
+    </row>
+    <row r="17" spans="1:10" ht="15">
+      <c r="A17" s="72"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="56"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="48" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="45">
-      <c r="A5" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="69" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="65" t="s">
-        <v>182</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30">
-      <c r="A6" s="64" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" s="60" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="59"/>
-      <c r="G6" s="67" t="s">
+      <c r="B18" s="49"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+    </row>
+    <row r="19" spans="1:10" ht="15">
+      <c r="A19" s="61"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J19" s="56"/>
+    </row>
+    <row r="20" spans="1:10" ht="15">
+      <c r="A20" s="61"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J20" s="56"/>
+    </row>
+    <row r="21" spans="1:10" ht="15">
+      <c r="A21" s="61"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J21" s="56"/>
+    </row>
+    <row r="22" spans="1:10" ht="15">
+      <c r="A22" s="61"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J22" s="56"/>
+    </row>
+    <row r="23" spans="1:10" ht="15">
+      <c r="A23" s="61"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J23" s="56"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+    </row>
+    <row r="25" spans="1:10" ht="15">
+      <c r="A25" s="61"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J25" s="59"/>
+    </row>
+    <row r="26" spans="1:10" ht="15">
+      <c r="A26" s="61"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="59"/>
+    </row>
+    <row r="27" spans="1:10" ht="15">
+      <c r="A27" s="61"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J27" s="59"/>
+    </row>
+    <row r="28" spans="1:10" ht="15">
+      <c r="A28" s="61"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="59"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+    </row>
+    <row r="30" spans="1:10" ht="15">
+      <c r="A30" s="61"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" s="59"/>
+    </row>
+    <row r="31" spans="1:10" ht="15">
+      <c r="A31" s="61"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J31" s="59"/>
+    </row>
+    <row r="32" spans="1:10" ht="15">
+      <c r="A32" s="61"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J32" s="59"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="H6" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="I6" s="70" t="s">
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+    </row>
+    <row r="34" spans="1:10" ht="15">
+      <c r="A34" s="72"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="75"/>
+      <c r="I34" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J34" s="72"/>
+    </row>
+    <row r="35" spans="1:10" ht="15">
+      <c r="A35" s="72"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="75"/>
+      <c r="I35" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J35" s="72"/>
+    </row>
+    <row r="36" spans="1:10" ht="15">
+      <c r="A36" s="72"/>
+      <c r="B36" s="73"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="75"/>
+      <c r="I36" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J36" s="72"/>
+    </row>
+    <row r="37" spans="1:10" ht="15">
+      <c r="A37" s="72"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="75"/>
+      <c r="I37" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J37" s="72"/>
+    </row>
+    <row r="38" spans="1:10" ht="15">
+      <c r="A38" s="72"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="72"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J38" s="72"/>
+    </row>
+    <row r="39" spans="1:10" ht="15">
+      <c r="A39" s="72"/>
+      <c r="B39" s="73"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="72"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J39" s="72"/>
+    </row>
+    <row r="40" spans="1:10" ht="15">
+      <c r="A40" s="72"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J40" s="72"/>
+    </row>
+    <row r="41" spans="1:10" ht="15">
+      <c r="A41" s="72"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="J41" s="72"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="48" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="45">
-      <c r="A7" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="68" t="s">
-        <v>177</v>
-      </c>
-      <c r="H7" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30">
-      <c r="A8" s="64" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>171</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="67" t="s">
+      <c r="B42" s="49"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+    </row>
+    <row r="43" spans="1:10" ht="15">
+      <c r="A43" s="72"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="H8" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30">
-      <c r="A9" s="64" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" s="60" t="s">
-        <v>185</v>
-      </c>
-      <c r="C9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>194</v>
-      </c>
-      <c r="H9" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="I9" s="61" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-    </row>
-    <row r="11" spans="1:9" ht="15">
-      <c r="A11" s="64"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I11" s="58"/>
-    </row>
-    <row r="12" spans="1:9" ht="15">
-      <c r="A12" s="64"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I12" s="58"/>
-    </row>
-    <row r="13" spans="1:9" ht="15">
-      <c r="A13" s="64"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I13" s="58"/>
-    </row>
-    <row r="14" spans="1:9" ht="15">
-      <c r="A14" s="64"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I14" s="58"/>
-    </row>
-    <row r="15" spans="1:9" ht="15">
-      <c r="A15" s="64"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I15" s="58"/>
-    </row>
-    <row r="16" spans="1:9" ht="15">
-      <c r="A16" s="64"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I16" s="58"/>
-    </row>
-    <row r="17" spans="1:9" ht="15">
-      <c r="A17" s="64"/>
-      <c r="B17" s="72"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I17" s="58"/>
-    </row>
-    <row r="18" spans="1:9" ht="15">
-      <c r="A18" s="64"/>
-      <c r="B18" s="72"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62" t="s">
-        <v>193</v>
-      </c>
-      <c r="I18" s="58"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="48" t="s">
-        <v>188</v>
-      </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-    </row>
-    <row r="20" spans="1:9" ht="60">
-      <c r="A20" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="72" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="75" t="s">
-        <v>191</v>
-      </c>
-      <c r="H20" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I20" s="58" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15">
-      <c r="A21" s="64"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I21" s="58"/>
-    </row>
-    <row r="22" spans="1:9" ht="15">
-      <c r="A22" s="64"/>
-      <c r="B22" s="72"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I22" s="58"/>
-    </row>
-    <row r="23" spans="1:9" ht="15">
-      <c r="A23" s="64"/>
-      <c r="B23" s="72"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I23" s="58"/>
-    </row>
-    <row r="24" spans="1:9" ht="15">
-      <c r="A24" s="64"/>
-      <c r="B24" s="72"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I24" s="58"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="48" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="49"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-    </row>
-    <row r="26" spans="1:9" ht="30">
-      <c r="A26" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="72" t="s">
-        <v>206</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="62"/>
-      <c r="G26" s="75" t="s">
-        <v>208</v>
-      </c>
-      <c r="H26" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I26" s="62" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="45">
-      <c r="A27" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="72" t="s">
-        <v>209</v>
-      </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="75" t="s">
-        <v>211</v>
-      </c>
-      <c r="H27" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I27" s="62" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="45">
-      <c r="A28" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="C28" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="75" t="s">
-        <v>213</v>
-      </c>
-      <c r="H28" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I28" s="62" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15">
-      <c r="A29" s="64"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="62"/>
-    </row>
-    <row r="30" spans="1:9" ht="15">
-      <c r="A30" s="64"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="62"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-    </row>
-    <row r="32" spans="1:9" ht="30">
-      <c r="A32" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="72" t="s">
-        <v>199</v>
-      </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="75" t="s">
-        <v>201</v>
-      </c>
-      <c r="H32" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I32" s="62" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="45">
-      <c r="A33" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="72" t="s">
-        <v>202</v>
-      </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="75" t="s">
-        <v>203</v>
-      </c>
-      <c r="H33" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I33" s="62" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="30">
-      <c r="A34" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="75" t="s">
-        <v>203</v>
-      </c>
-      <c r="H34" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="I34" s="62" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="48" t="s">
-        <v>197</v>
-      </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="64"/>
-      <c r="B36" s="78"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="56"/>
-      <c r="F36" s="56"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="56"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="64"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="56"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" s="64"/>
-      <c r="B38" s="78"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="79"/>
-      <c r="I38" s="56"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="64"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="56"/>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="56"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="64"/>
-      <c r="B40" s="78"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="56"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="64"/>
-      <c r="B41" s="78"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="56"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="56"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="64"/>
-      <c r="B42" s="78"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="79"/>
-      <c r="H42" s="79"/>
-      <c r="I42" s="56"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="64"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="56"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="64"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="79"/>
-      <c r="H45" s="79"/>
-      <c r="I45" s="56"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="64"/>
-      <c r="B46" s="78"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="79"/>
-      <c r="H46" s="79"/>
-      <c r="I46" s="56"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="64"/>
-      <c r="B47" s="78"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="79"/>
-      <c r="H47" s="79"/>
-      <c r="I47" s="56"/>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="A48" s="64"/>
-      <c r="B48" s="78"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="79"/>
-      <c r="H48" s="79"/>
-      <c r="I48" s="56"/>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="64"/>
-      <c r="B49" s="78"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="79"/>
-      <c r="I49" s="56"/>
-    </row>
-    <row r="50" spans="1:9">
-      <c r="A50" s="64"/>
-      <c r="B50" s="78"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="79"/>
-      <c r="H50" s="79"/>
-      <c r="I50" s="56"/>
-    </row>
-    <row r="51" spans="1:9">
-      <c r="A51" s="64"/>
-      <c r="B51" s="78"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="79"/>
-      <c r="H51" s="79"/>
-      <c r="I51" s="56"/>
-    </row>
-    <row r="52" spans="1:9">
-      <c r="A52" s="64"/>
-      <c r="B52" s="78"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="79"/>
-      <c r="H52" s="79"/>
-      <c r="I52" s="56"/>
-    </row>
-    <row r="53" spans="1:9">
-      <c r="A53" s="64"/>
-      <c r="B53" s="78"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="56"/>
-    </row>
-    <row r="54" spans="1:9">
-      <c r="A54" s="64"/>
-      <c r="B54" s="78"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="79"/>
-      <c r="H54" s="79"/>
-      <c r="I54" s="56"/>
-    </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="64"/>
-      <c r="B55" s="78"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="79"/>
-      <c r="H55" s="79"/>
-      <c r="I55" s="56"/>
-    </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="64"/>
-      <c r="B56" s="78"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="79"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="56"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="64"/>
-      <c r="B57" s="78"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="56"/>
-      <c r="E57" s="56"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="79"/>
-      <c r="H57" s="79"/>
-      <c r="I57" s="56"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="64"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="56"/>
-      <c r="D58" s="56"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="79"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="56"/>
+      <c r="J43" s="72"/>
+    </row>
+    <row r="44" spans="1:10" ht="15">
+      <c r="A44" s="72"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J44" s="72"/>
+    </row>
+    <row r="45" spans="1:10" ht="15">
+      <c r="A45" s="72"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J45" s="72"/>
+    </row>
+    <row r="46" spans="1:10" ht="15">
+      <c r="A46" s="72"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J46" s="72"/>
+    </row>
+    <row r="47" spans="1:10" ht="15">
+      <c r="A47" s="72"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J47" s="72"/>
+    </row>
+    <row r="48" spans="1:10" ht="15">
+      <c r="A48" s="72"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="72"/>
+      <c r="D48" s="72"/>
+      <c r="E48" s="72"/>
+      <c r="F48" s="72"/>
+      <c r="G48" s="72"/>
+      <c r="H48" s="77"/>
+      <c r="I48" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J48" s="72"/>
+    </row>
+    <row r="49" spans="1:10" ht="15">
+      <c r="A49" s="72"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="77"/>
+      <c r="I49" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J49" s="72"/>
+    </row>
+    <row r="50" spans="1:10" ht="15">
+      <c r="A50" s="72"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72"/>
+      <c r="E50" s="72"/>
+      <c r="F50" s="72"/>
+      <c r="G50" s="72"/>
+      <c r="H50" s="77"/>
+      <c r="I50" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J50" s="72"/>
+    </row>
+    <row r="51" spans="1:10" ht="15">
+      <c r="A51" s="72"/>
+      <c r="B51" s="76"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
+      <c r="F51" s="72"/>
+      <c r="G51" s="72"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J51" s="72"/>
+    </row>
+    <row r="52" spans="1:10" ht="15">
+      <c r="A52" s="72"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="72"/>
+      <c r="F52" s="72"/>
+      <c r="G52" s="72"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J52" s="72"/>
+    </row>
+    <row r="53" spans="1:10" ht="15">
+      <c r="A53" s="72"/>
+      <c r="B53" s="76"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="72"/>
+      <c r="E53" s="72"/>
+      <c r="F53" s="72"/>
+      <c r="G53" s="72"/>
+      <c r="H53" s="77"/>
+      <c r="I53" s="71" t="s">
+        <v>172</v>
+      </c>
+      <c r="J53" s="72"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="A44:I44"/>
+  <mergeCells count="14">
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A18:J18"/>
     <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:H9">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOT VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H4)))</formula>
+  <conditionalFormatting sqref="I7:I8">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I7)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32:H34 H11:H18 H20:H24 H26:H30">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NOT VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H11)))</formula>
+  <conditionalFormatting sqref="I43:I1048576 I30:I32 I10:I17 I19:I23 I25:I28 I34:I41 I4:I6">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("VERIFIED",H11)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",I4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"NOT VERIFIED"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36:H43 H45:H1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NOT VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",H36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="VERIFIED">
-      <formula>NOT(ISERROR(SEARCH("VERIFIED",H36)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
       <formula>"NOT VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added mission requirement sub-requirements for calculating, recording, and sending relative distance data
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="215">
   <si>
     <t>Document Title</t>
   </si>
@@ -662,9 +662,6 @@
     <t>Verification Mission Stage</t>
   </si>
   <si>
-    <t>Launch Requirements</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -674,9 +671,6 @@
     <t>Mission Operations Requirements</t>
   </si>
   <si>
-    <t>ODAR Requirements</t>
-  </si>
-  <si>
     <t>Communication Requirements</t>
   </si>
   <si>
@@ -734,10 +728,73 @@
     <t>Cost</t>
   </si>
   <si>
+    <t>RCL-RFP-1</t>
+  </si>
+  <si>
     <t>Architecture Requirements</t>
   </si>
   <si>
     <t>RCL-ARC1</t>
+  </si>
+  <si>
+    <t>The mission will consist of two identical spacecraft</t>
+  </si>
+  <si>
+    <t>Risk Mitigation</t>
+  </si>
+  <si>
+    <t>RCL-ARC2</t>
+  </si>
+  <si>
+    <t>Architecture Sub-Requirements</t>
+  </si>
+  <si>
+    <t>The two spacecraft must be able to integrate into the same dispenser</t>
+  </si>
+  <si>
+    <t>Launch Requirement</t>
+  </si>
+  <si>
+    <t>RCL-ARC2-1</t>
+  </si>
+  <si>
+    <t>RCL-ARC2-2</t>
+  </si>
+  <si>
+    <t>The two spacecraft will be conjoined for integration into dispenser</t>
+  </si>
+  <si>
+    <t>The two spacecraft will be capable of separating in orbit</t>
+  </si>
+  <si>
+    <t>Mission Requirements</t>
+  </si>
+  <si>
+    <t>The spacecraft must be capable of determining relative distance between it and a resident space object</t>
+  </si>
+  <si>
+    <t>Mission Operations Requiremetns</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-1</t>
+  </si>
+  <si>
+    <t>Top Level Sub-Requirements</t>
+  </si>
+  <si>
+    <t>The spacecraft must be capable of recording relative distance between it and a resident space object</t>
+  </si>
+  <si>
+    <t>The spacecraft must be capable of relaying relative distance between it and a resident space object to the ground</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-2</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-3</t>
+  </si>
+  <si>
+    <t>Mission Operations Sub-Requirements</t>
   </si>
 </sst>
 </file>
@@ -4405,10 +4462,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4437,16 +4494,16 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>53</v>
       </c>
       <c r="I1" s="50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J1" s="52" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25">
@@ -4488,21 +4545,21 @@
         <v>167</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
       <c r="E4" s="72"/>
       <c r="F4" s="72"/>
       <c r="G4" s="72" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H4" s="77"/>
       <c r="I4" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J4" s="72" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45">
@@ -4510,21 +4567,21 @@
         <v>167</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C5" s="72"/>
       <c r="D5" s="72"/>
       <c r="E5" s="72"/>
       <c r="F5" s="72"/>
       <c r="G5" s="72" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H5" s="77"/>
       <c r="I5" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J5" s="72" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45">
@@ -4532,21 +4589,21 @@
         <v>167</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C6" s="72"/>
       <c r="D6" s="72"/>
       <c r="E6" s="72"/>
       <c r="F6" s="72"/>
       <c r="G6" s="72" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H6" s="77"/>
       <c r="I6" s="71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J6" s="72" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45">
@@ -4554,21 +4611,21 @@
         <v>167</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="57"/>
       <c r="F7" s="57"/>
       <c r="G7" s="63" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H7" s="63"/>
       <c r="I7" s="62" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J7" s="64" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
@@ -4576,26 +4633,26 @@
         <v>167</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="57"/>
       <c r="F8" s="57"/>
       <c r="G8" s="63" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H8" s="63"/>
       <c r="I8" s="62" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J8" s="64" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
@@ -4609,167 +4666,221 @@
     </row>
     <row r="10" spans="1:10" ht="15">
       <c r="A10" s="72" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="65" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
       <c r="G10" s="59" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H10" s="59"/>
       <c r="I10" s="59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J10" s="56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15">
       <c r="A11" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="66" t="s">
+        <v>195</v>
+      </c>
       <c r="C11" s="59"/>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
+      <c r="G11" s="59" t="s">
+        <v>196</v>
+      </c>
       <c r="H11" s="59"/>
       <c r="I11" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J11" s="56"/>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="A12" s="72"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J12" s="56"/>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="72"/>
-      <c r="B13" s="65"/>
+        <v>171</v>
+      </c>
+      <c r="J11" s="56" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A13" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="65" t="s">
+        <v>199</v>
+      </c>
       <c r="C13" s="59"/>
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J13" s="56"/>
-    </row>
-    <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="72"/>
-      <c r="B14" s="65"/>
+      <c r="G13" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J13" s="56" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1">
+      <c r="A14" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>203</v>
+      </c>
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
       <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J14" s="56"/>
+      <c r="G14" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J14" s="56" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="72"/>
-      <c r="B15" s="65"/>
+      <c r="A15" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>204</v>
+      </c>
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
       <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J15" s="56"/>
-    </row>
-    <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="72"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J16" s="56"/>
-    </row>
-    <row r="17" spans="1:10" ht="15">
-      <c r="A17" s="72"/>
-      <c r="B17" s="65"/>
+      <c r="G15" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>206</v>
+      </c>
       <c r="C17" s="59"/>
       <c r="D17" s="59"/>
       <c r="E17" s="59"/>
       <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59" t="s">
+      <c r="G17" s="68" t="s">
+        <v>207</v>
+      </c>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J17" s="59" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30">
+      <c r="A18" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="65" t="s">
+        <v>210</v>
+      </c>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="68" t="s">
         <v>172</v>
       </c>
-      <c r="J17" s="56"/>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-    </row>
-    <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="61"/>
-      <c r="B19" s="65"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J18" s="59" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30">
+      <c r="A19" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="65" t="s">
+        <v>211</v>
+      </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
+      <c r="G19" s="68" t="s">
+        <v>172</v>
+      </c>
       <c r="H19" s="68"/>
       <c r="I19" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J19" s="56"/>
-    </row>
-    <row r="20" spans="1:10" ht="15">
-      <c r="A20" s="61"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J20" s="56"/>
+        <v>171</v>
+      </c>
+      <c r="J19" s="59" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
     </row>
     <row r="21" spans="1:10" ht="15">
       <c r="A21" s="61"/>
@@ -4781,189 +4892,189 @@
       <c r="G21" s="59"/>
       <c r="H21" s="68"/>
       <c r="I21" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J21" s="56"/>
-    </row>
-    <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="61"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J22" s="56"/>
+        <v>171</v>
+      </c>
+      <c r="J21" s="59"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="61"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="68"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J23" s="56"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
+        <v>171</v>
+      </c>
+      <c r="J23" s="72"/>
+    </row>
+    <row r="24" spans="1:10" ht="15">
+      <c r="A24" s="72"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J24" s="72"/>
     </row>
     <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="61"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="68"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="73"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J25" s="59"/>
+        <v>171</v>
+      </c>
+      <c r="J25" s="72"/>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="61"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="68"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="75"/>
       <c r="I26" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J26" s="59"/>
+        <v>171</v>
+      </c>
+      <c r="J26" s="72"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="61"/>
-      <c r="B27" s="65"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="68"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="73"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="75"/>
       <c r="I27" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J27" s="59"/>
+        <v>171</v>
+      </c>
+      <c r="J27" s="72"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="61"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="68"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="73"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J28" s="59"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="72"/>
+    </row>
+    <row r="29" spans="1:10" ht="15">
+      <c r="A29" s="72"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" s="72"/>
+    </row>
+    <row r="30" spans="1:10" ht="15">
+      <c r="A30" s="72"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J30" s="72"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-    </row>
-    <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="61"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J30" s="59"/>
-    </row>
-    <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="61"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J31" s="59"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="61"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="J32" s="59"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J32" s="72"/>
+    </row>
+    <row r="33" spans="1:10" ht="15">
+      <c r="A33" s="72"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J33" s="72"/>
     </row>
     <row r="34" spans="1:10" ht="15">
       <c r="A34" s="72"/>
-      <c r="B34" s="73"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="72"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="68" t="s">
-        <v>172</v>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J34" s="72"/>
     </row>
@@ -4975,274 +5086,120 @@
       <c r="E35" s="72"/>
       <c r="F35" s="72"/>
       <c r="G35" s="72"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="68" t="s">
-        <v>172</v>
+      <c r="H35" s="77"/>
+      <c r="I35" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J35" s="72"/>
     </row>
     <row r="36" spans="1:10" ht="15">
       <c r="A36" s="72"/>
-      <c r="B36" s="73"/>
+      <c r="B36" s="76"/>
       <c r="C36" s="72"/>
       <c r="D36" s="72"/>
       <c r="E36" s="72"/>
       <c r="F36" s="72"/>
       <c r="G36" s="72"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="68" t="s">
-        <v>172</v>
+      <c r="H36" s="77"/>
+      <c r="I36" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J36" s="72"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="72"/>
-      <c r="B37" s="73"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="72"/>
       <c r="D37" s="72"/>
       <c r="E37" s="72"/>
       <c r="F37" s="72"/>
       <c r="G37" s="72"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="68" t="s">
-        <v>172</v>
+      <c r="H37" s="77"/>
+      <c r="I37" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J37" s="72"/>
     </row>
     <row r="38" spans="1:10" ht="15">
       <c r="A38" s="72"/>
-      <c r="B38" s="73"/>
+      <c r="B38" s="76"/>
       <c r="C38" s="72"/>
       <c r="D38" s="72"/>
       <c r="E38" s="72"/>
       <c r="F38" s="72"/>
       <c r="G38" s="72"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="68" t="s">
-        <v>172</v>
+      <c r="H38" s="77"/>
+      <c r="I38" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J38" s="72"/>
     </row>
     <row r="39" spans="1:10" ht="15">
       <c r="A39" s="72"/>
-      <c r="B39" s="73"/>
+      <c r="B39" s="76"/>
       <c r="C39" s="72"/>
       <c r="D39" s="72"/>
       <c r="E39" s="72"/>
       <c r="F39" s="72"/>
       <c r="G39" s="72"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="68" t="s">
-        <v>172</v>
+      <c r="H39" s="77"/>
+      <c r="I39" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J39" s="72"/>
     </row>
     <row r="40" spans="1:10" ht="15">
       <c r="A40" s="72"/>
-      <c r="B40" s="73"/>
+      <c r="B40" s="76"/>
       <c r="C40" s="72"/>
       <c r="D40" s="72"/>
       <c r="E40" s="72"/>
       <c r="F40" s="72"/>
       <c r="G40" s="72"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="68" t="s">
-        <v>172</v>
+      <c r="H40" s="77"/>
+      <c r="I40" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J40" s="72"/>
     </row>
     <row r="41" spans="1:10" ht="15">
       <c r="A41" s="72"/>
-      <c r="B41" s="73"/>
+      <c r="B41" s="76"/>
       <c r="C41" s="72"/>
       <c r="D41" s="72"/>
       <c r="E41" s="72"/>
       <c r="F41" s="72"/>
       <c r="G41" s="72"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="68" t="s">
-        <v>172</v>
+      <c r="H41" s="77"/>
+      <c r="I41" s="71" t="s">
+        <v>171</v>
       </c>
       <c r="J41" s="72"/>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="48" t="s">
-        <v>176</v>
-      </c>
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49"/>
-    </row>
-    <row r="43" spans="1:10" ht="15">
-      <c r="A43" s="72"/>
-      <c r="B43" s="76"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J43" s="72"/>
-    </row>
-    <row r="44" spans="1:10" ht="15">
-      <c r="A44" s="72"/>
-      <c r="B44" s="76"/>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J44" s="72"/>
-    </row>
-    <row r="45" spans="1:10" ht="15">
-      <c r="A45" s="72"/>
-      <c r="B45" s="76"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="77"/>
-      <c r="I45" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J45" s="72"/>
-    </row>
-    <row r="46" spans="1:10" ht="15">
-      <c r="A46" s="72"/>
-      <c r="B46" s="76"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="77"/>
-      <c r="I46" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J46" s="72"/>
-    </row>
-    <row r="47" spans="1:10" ht="15">
-      <c r="A47" s="72"/>
-      <c r="B47" s="76"/>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J47" s="72"/>
-    </row>
-    <row r="48" spans="1:10" ht="15">
-      <c r="A48" s="72"/>
-      <c r="B48" s="76"/>
-      <c r="C48" s="72"/>
-      <c r="D48" s="72"/>
-      <c r="E48" s="72"/>
-      <c r="F48" s="72"/>
-      <c r="G48" s="72"/>
-      <c r="H48" s="77"/>
-      <c r="I48" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J48" s="72"/>
-    </row>
-    <row r="49" spans="1:10" ht="15">
-      <c r="A49" s="72"/>
-      <c r="B49" s="76"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="72"/>
-      <c r="E49" s="72"/>
-      <c r="F49" s="72"/>
-      <c r="G49" s="72"/>
-      <c r="H49" s="77"/>
-      <c r="I49" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J49" s="72"/>
-    </row>
-    <row r="50" spans="1:10" ht="15">
-      <c r="A50" s="72"/>
-      <c r="B50" s="76"/>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
-      <c r="E50" s="72"/>
-      <c r="F50" s="72"/>
-      <c r="G50" s="72"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J50" s="72"/>
-    </row>
-    <row r="51" spans="1:10" ht="15">
-      <c r="A51" s="72"/>
-      <c r="B51" s="76"/>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J51" s="72"/>
-    </row>
-    <row r="52" spans="1:10" ht="15">
-      <c r="A52" s="72"/>
-      <c r="B52" s="76"/>
-      <c r="C52" s="72"/>
-      <c r="D52" s="72"/>
-      <c r="E52" s="72"/>
-      <c r="F52" s="72"/>
-      <c r="G52" s="72"/>
-      <c r="H52" s="77"/>
-      <c r="I52" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J52" s="72"/>
-    </row>
-    <row r="53" spans="1:10" ht="15">
-      <c r="A53" s="72"/>
-      <c r="B53" s="76"/>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
-      <c r="E53" s="72"/>
-      <c r="F53" s="72"/>
-      <c r="G53" s="72"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="71" t="s">
-        <v>172</v>
-      </c>
-      <c r="J53" s="72"/>
+    <row r="42" spans="1:10" ht="15">
+      <c r="A42" s="72"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="77"/>
+      <c r="I42" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J42" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A31:J31"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A12:J12"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
@@ -5258,7 +5215,7 @@
       <formula>"VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I43:I1048576 I30:I32 I10:I17 I19:I23 I25:I28 I34:I41 I4:I6">
+  <conditionalFormatting sqref="I32:I1048576 I21 I23:I30 I4:I6 I13:I15 I10:I11 I17:I19">
     <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NOT VERIFIED">
       <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I4)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added ADC reuqirmement as well as Propulsion and Power subsystems
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="226">
   <si>
     <t>Document Title</t>
   </si>
@@ -795,6 +795,39 @@
   </si>
   <si>
     <t>Mission Operations Sub-Requirements</t>
+  </si>
+  <si>
+    <t>Mission Operations Requirment</t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize a Command and Data Handling Subsystem to fulfill requirement RCL-MOP1-2</t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize a Communications Subysystem to fulfill requirement RCL-MOP1-3</t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize a Propulsion Subsystem</t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize a Power Subsystem</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-2-CDH</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-3-COM</t>
+  </si>
+  <si>
+    <t>RCL-MOP2-PWR</t>
+  </si>
+  <si>
+    <t>RCL-RFP-PRP</t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize an Attitude Determination and Control Subsystem to fulfill requirement RCL-MOP1-1</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-1-ADC</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1432,7 @@
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="14">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1421,6 +1454,114 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4462,10 +4603,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4868,37 +5009,53 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-    </row>
-    <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="61"/>
-      <c r="B21" s="65"/>
+    <row r="20" spans="1:10" ht="15">
+      <c r="A20" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="65" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J20" s="59" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30">
+      <c r="A21" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>219</v>
+      </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
       <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
+      <c r="G21" s="68" t="s">
+        <v>172</v>
+      </c>
       <c r="H21" s="68"/>
       <c r="I21" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J21" s="59"/>
+      <c r="J21" s="59" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="48" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
@@ -4910,84 +5067,108 @@
       <c r="I22" s="49"/>
       <c r="J22" s="49"/>
     </row>
-    <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="72"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="75"/>
+    <row r="23" spans="1:10" ht="30">
+      <c r="A23" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="65" t="s">
+        <v>224</v>
+      </c>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="68" t="s">
+        <v>215</v>
+      </c>
+      <c r="H23" s="68"/>
       <c r="I23" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J23" s="72"/>
-    </row>
-    <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="72"/>
-      <c r="B24" s="76"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="75"/>
+      <c r="J23" s="59" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30">
+      <c r="A24" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="65" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="H24" s="68"/>
       <c r="I24" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J24" s="72"/>
-    </row>
-    <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="72"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="75"/>
+      <c r="J24" s="59" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="30">
+      <c r="A25" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="H25" s="68"/>
       <c r="I25" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J25" s="72"/>
+      <c r="J25" s="59" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="72"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="75"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="68"/>
       <c r="I26" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J26" s="72"/>
-    </row>
-    <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="72"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="J27" s="72"/>
+      <c r="J26" s="59"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="49"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
     </row>
     <row r="28" spans="1:10" ht="15">
       <c r="A28" s="72"/>
       <c r="B28" s="73"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
       <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
       <c r="H28" s="75"/>
       <c r="I28" s="68" t="s">
         <v>171</v>
@@ -4996,7 +5177,7 @@
     </row>
     <row r="29" spans="1:10" ht="15">
       <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="72"/>
       <c r="D29" s="72"/>
       <c r="E29" s="72"/>
@@ -5022,89 +5203,89 @@
       </c>
       <c r="J30" s="72"/>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
+    <row r="31" spans="1:10" ht="15">
+      <c r="A31" s="72"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J31" s="72"/>
     </row>
     <row r="32" spans="1:10" ht="15">
       <c r="A32" s="72"/>
-      <c r="B32" s="76"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="72"/>
       <c r="D32" s="72"/>
       <c r="E32" s="72"/>
       <c r="F32" s="72"/>
       <c r="G32" s="72"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="71" t="s">
+      <c r="H32" s="75"/>
+      <c r="I32" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J32" s="72"/>
     </row>
     <row r="33" spans="1:10" ht="15">
       <c r="A33" s="72"/>
-      <c r="B33" s="76"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="72"/>
       <c r="D33" s="72"/>
       <c r="E33" s="72"/>
       <c r="F33" s="72"/>
       <c r="G33" s="72"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="71" t="s">
+      <c r="H33" s="75"/>
+      <c r="I33" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J33" s="72"/>
     </row>
     <row r="34" spans="1:10" ht="15">
       <c r="A34" s="72"/>
-      <c r="B34" s="76"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="72"/>
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
       <c r="F34" s="72"/>
       <c r="G34" s="72"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="71" t="s">
+      <c r="H34" s="75"/>
+      <c r="I34" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J34" s="72"/>
     </row>
     <row r="35" spans="1:10" ht="15">
       <c r="A35" s="72"/>
-      <c r="B35" s="76"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="72"/>
       <c r="D35" s="72"/>
       <c r="E35" s="72"/>
       <c r="F35" s="72"/>
       <c r="G35" s="72"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="71" t="s">
+      <c r="H35" s="75"/>
+      <c r="I35" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J35" s="72"/>
     </row>
-    <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="72"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J36" s="72"/>
+    <row r="36" spans="1:10">
+      <c r="A36" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="72"/>
@@ -5190,12 +5371,82 @@
       </c>
       <c r="J42" s="72"/>
     </row>
+    <row r="43" spans="1:10" ht="15">
+      <c r="A43" s="72"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J43" s="72"/>
+    </row>
+    <row r="44" spans="1:10" ht="15">
+      <c r="A44" s="72"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="72"/>
+      <c r="G44" s="72"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J44" s="72"/>
+    </row>
+    <row r="45" spans="1:10" ht="15">
+      <c r="A45" s="72"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="77"/>
+      <c r="I45" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J45" s="72"/>
+    </row>
+    <row r="46" spans="1:10" ht="15">
+      <c r="A46" s="72"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
+      <c r="E46" s="72"/>
+      <c r="F46" s="72"/>
+      <c r="G46" s="72"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J46" s="72"/>
+    </row>
+    <row r="47" spans="1:10" ht="15">
+      <c r="A47" s="72"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J47" s="72"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A20:J20"/>
     <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A36:J36"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A9:J9"/>
@@ -5208,21 +5459,21 @@
     <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:I8">
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="NOT VERIFIED">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOT VERIFIED">
       <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I7)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32:I1048576 I21 I23:I30 I4:I6 I13:I15 I10:I11 I17:I19">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NOT VERIFIED">
+  <conditionalFormatting sqref="I37:I1048576 I28:I35 I4:I6 I13:I15 I10:I11 I23:I26 I17:I21">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NOT VERIFIED">
       <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="VERIFIED">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="VERIFIED">
       <formula>NOT(ISERROR(SEARCH("VERIFIED",I4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"NOT VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Power Requirements and reorganized structures requirements
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="238">
   <si>
     <t>Document Title</t>
   </si>
@@ -671,10 +671,7 @@
     <t>Mission Operations Requirements</t>
   </si>
   <si>
-    <t>Communication Requirements</t>
-  </si>
-  <si>
-    <t>RFP Requirements</t>
+    <t>Power Requirements</t>
   </si>
   <si>
     <t>Task Number Taxonomy</t>
@@ -695,21 +692,6 @@
     <t>A method of verifying the successful completion of each mission requirement shall be incorperated into the spacecraft design and mission operations procedures</t>
   </si>
   <si>
-    <t>RCL-RFP1-x</t>
-  </si>
-  <si>
-    <t>RCL-RFP2-x</t>
-  </si>
-  <si>
-    <t>RCL-RFP3-x</t>
-  </si>
-  <si>
-    <t>RCL-MOP1-x</t>
-  </si>
-  <si>
-    <t>RCL-MOP2-x</t>
-  </si>
-  <si>
     <t>Rationale</t>
   </si>
   <si>
@@ -728,39 +710,18 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>RCL-RFP-1</t>
-  </si>
-  <si>
-    <t>Architecture Requirements</t>
-  </si>
-  <si>
-    <t>RCL-ARC1</t>
-  </si>
-  <si>
     <t>The mission will consist of two identical spacecraft</t>
   </si>
   <si>
     <t>Risk Mitigation</t>
   </si>
   <si>
-    <t>RCL-ARC2</t>
-  </si>
-  <si>
-    <t>Architecture Sub-Requirements</t>
-  </si>
-  <si>
     <t>The two spacecraft must be able to integrate into the same dispenser</t>
   </si>
   <si>
     <t>Launch Requirement</t>
   </si>
   <si>
-    <t>RCL-ARC2-1</t>
-  </si>
-  <si>
-    <t>RCL-ARC2-2</t>
-  </si>
-  <si>
     <t>The two spacecraft will be conjoined for integration into dispenser</t>
   </si>
   <si>
@@ -800,15 +761,6 @@
     <t>Mission Operations Requirment</t>
   </si>
   <si>
-    <t>The spacecraft will utilize a Command and Data Handling Subsystem to fulfill requirement RCL-MOP1-2</t>
-  </si>
-  <si>
-    <t>The spacecraft will utilize a Communications Subysystem to fulfill requirement RCL-MOP1-3</t>
-  </si>
-  <si>
-    <t>The spacecraft will utilize a Propulsion Subsystem</t>
-  </si>
-  <si>
     <t>The spacecraft will utilize a Power Subsystem</t>
   </si>
   <si>
@@ -824,10 +776,94 @@
     <t>RCL-RFP-PRP</t>
   </si>
   <si>
-    <t>The spacecraft will utilize an Attitude Determination and Control Subsystem to fulfill requirement RCL-MOP1-1</t>
-  </si>
-  <si>
     <t>RCL-MOP1-1-ADC</t>
+  </si>
+  <si>
+    <t>Structure System</t>
+  </si>
+  <si>
+    <t>Structure Sub-Requirements</t>
+  </si>
+  <si>
+    <t>RCL-STR</t>
+  </si>
+  <si>
+    <t>RCL-STR-1</t>
+  </si>
+  <si>
+    <t>RCL-STR-2</t>
+  </si>
+  <si>
+    <t>RCL-STR-3</t>
+  </si>
+  <si>
+    <t>RCL-STR-4</t>
+  </si>
+  <si>
+    <t>RCL-STR-5</t>
+  </si>
+  <si>
+    <t>RCL-RFP1</t>
+  </si>
+  <si>
+    <t>RCL-RFP2</t>
+  </si>
+  <si>
+    <t>RCL-RFP3</t>
+  </si>
+  <si>
+    <t>RCL-MOP1</t>
+  </si>
+  <si>
+    <t>RCL-MOP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The spacecraft will utilize a Propulsion Subsystem </t>
+  </si>
+  <si>
+    <t>RFP Requirements 1-3</t>
+  </si>
+  <si>
+    <t>Mission Operations Requirement 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The spacecraft will utilize an Attitude Determination and Control Subsystem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The spacecraft will utilize a Command and Data Handling Subsystem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The spacecraft will utilize a Communications Subysystem </t>
+  </si>
+  <si>
+    <t>The spacecraft will utilize a Structures Subsystem</t>
+  </si>
+  <si>
+    <t>The power subsystem will utilize an Electircal Power System to manager power distribution to each subsystem of the spacecraft</t>
+  </si>
+  <si>
+    <t>The power subsystem will utilize a rechargable battery to store power for each subystem of the spacecraft</t>
+  </si>
+  <si>
+    <t>RCL-MOP2-PWR1</t>
+  </si>
+  <si>
+    <t>RCL-MOP2-PWR2</t>
+  </si>
+  <si>
+    <t>RCL-MOP2-PWR3</t>
+  </si>
+  <si>
+    <t>The power subystem will utilize solar panels to generate a sufficient amount of power to compensate for the energy consumption of each subsystem of the spacecraft</t>
+  </si>
+  <si>
+    <t>RCL-MOP2-PWR4</t>
+  </si>
+  <si>
+    <t>A power budget will be created to ensure a net positive power marigin per orbit</t>
+  </si>
+  <si>
+    <t>Attitude Determination and Control Requirements</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1427,12 +1463,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1490,6 +1527,42 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4603,10 +4676,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4614,7 +4687,7 @@
     <col min="1" max="1" width="25" style="67" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60.28515625" style="70" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="53"/>
-    <col min="7" max="7" width="18.5703125" style="53" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="53" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" style="69" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" style="69" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" style="53" bestFit="1" customWidth="1"/>
@@ -4635,7 +4708,7 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="50" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>53</v>
@@ -4644,7 +4717,7 @@
         <v>170</v>
       </c>
       <c r="J1" s="52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25">
@@ -4686,21 +4759,21 @@
         <v>167</v>
       </c>
       <c r="B4" s="76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
       <c r="E4" s="72"/>
       <c r="F4" s="72"/>
       <c r="G4" s="72" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H4" s="77"/>
-      <c r="I4" s="71" t="s">
+      <c r="I4" s="77" t="s">
         <v>171</v>
       </c>
       <c r="J4" s="72" t="s">
-        <v>181</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="45">
@@ -4708,21 +4781,21 @@
         <v>167</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C5" s="72"/>
       <c r="D5" s="72"/>
       <c r="E5" s="72"/>
       <c r="F5" s="72"/>
       <c r="G5" s="72" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H5" s="77"/>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="77" t="s">
         <v>171</v>
       </c>
       <c r="J5" s="72" t="s">
-        <v>182</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45">
@@ -4730,21 +4803,21 @@
         <v>167</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="72"/>
       <c r="D6" s="72"/>
       <c r="E6" s="72"/>
       <c r="F6" s="72"/>
       <c r="G6" s="72" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H6" s="77"/>
-      <c r="I6" s="71" t="s">
+      <c r="I6" s="77" t="s">
         <v>171</v>
       </c>
       <c r="J6" s="72" t="s">
-        <v>183</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45">
@@ -4752,21 +4825,21 @@
         <v>167</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="57"/>
       <c r="F7" s="57"/>
       <c r="G7" s="63" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H7" s="63"/>
       <c r="I7" s="62" t="s">
         <v>171</v>
       </c>
       <c r="J7" s="64" t="s">
-        <v>184</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
@@ -4774,26 +4847,26 @@
         <v>167</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="57"/>
       <c r="F8" s="57"/>
       <c r="G8" s="63" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H8" s="63"/>
       <c r="I8" s="62" t="s">
         <v>171</v>
       </c>
       <c r="J8" s="64" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="48" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
@@ -4805,186 +4878,186 @@
       <c r="I9" s="49"/>
       <c r="J9" s="49"/>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="72" t="s">
-        <v>178</v>
-      </c>
-      <c r="B10" s="65" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59" t="s">
-        <v>191</v>
-      </c>
-      <c r="H10" s="59"/>
+        <v>14</v>
+      </c>
+      <c r="B10" s="73" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="77" t="s">
+        <v>182</v>
+      </c>
+      <c r="H10" s="79"/>
       <c r="I10" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="J10" s="56" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="A11" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="66" t="s">
-        <v>195</v>
-      </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59" t="s">
+      <c r="J10" s="72" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+    </row>
+    <row r="12" spans="1:10" ht="15">
+      <c r="A12" s="72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="J11" s="56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="49"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+      <c r="J12" s="56" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15">
       <c r="A13" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="65" t="s">
-        <v>199</v>
+      <c r="B13" s="66" t="s">
+        <v>186</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="59"/>
       <c r="E13" s="59"/>
       <c r="F13" s="59"/>
       <c r="G13" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59" t="s">
         <v>171</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="72" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
       <c r="F14" s="59"/>
       <c r="G14" s="59" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="H14" s="68"/>
       <c r="I14" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J14" s="56" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1">
       <c r="A15" s="72" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
       <c r="F15" s="59"/>
       <c r="G15" s="59" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="H15" s="68"/>
       <c r="I15" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J15" s="56" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15">
+      <c r="A16" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" s="48" t="s">
-        <v>209</v>
-      </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-    </row>
-    <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="65" t="s">
-        <v>206</v>
-      </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="68" t="s">
-        <v>207</v>
-      </c>
-      <c r="H17" s="68"/>
-      <c r="I17" s="68" t="s">
+      <c r="H16" s="68"/>
+      <c r="I16" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J17" s="59" t="s">
-        <v>208</v>
-      </c>
+      <c r="J16" s="56" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="59"/>
       <c r="E18" s="59"/>
       <c r="F18" s="59"/>
       <c r="G18" s="68" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="H18" s="68"/>
       <c r="I18" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J18" s="59" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
@@ -4992,7 +5065,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
@@ -5006,29 +5079,29 @@
         <v>171</v>
       </c>
       <c r="J19" s="59" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30">
       <c r="A20" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="C20" s="59"/>
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
       <c r="F20" s="59"/>
       <c r="G20" s="68" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="H20" s="68"/>
       <c r="I20" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J20" s="59" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30">
@@ -5036,79 +5109,79 @@
         <v>14</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
       <c r="F21" s="59"/>
       <c r="G21" s="68" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
       <c r="H21" s="68"/>
       <c r="I21" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J21" s="59" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="48" t="s">
-        <v>214</v>
-      </c>
-      <c r="B22" s="49"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-    </row>
-    <row r="23" spans="1:10" ht="30">
-      <c r="A23" s="61" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30">
+      <c r="A22" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="B22" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="68" t="s">
         <v>224</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="68" t="s">
-        <v>215</v>
-      </c>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68" t="s">
+      <c r="H22" s="68"/>
+      <c r="I22" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J23" s="59" t="s">
-        <v>225</v>
-      </c>
+      <c r="J22" s="59" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
     </row>
     <row r="24" spans="1:10" ht="30">
       <c r="A24" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="65" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
       <c r="G24" s="68" t="s">
-        <v>188</v>
+        <v>202</v>
       </c>
       <c r="H24" s="68"/>
       <c r="I24" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J24" s="59" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30">
@@ -5116,36 +5189,44 @@
         <v>14</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
       <c r="G25" s="68" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="H25" s="68"/>
       <c r="I25" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J25" s="59" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="61"/>
-      <c r="B26" s="65"/>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30">
+      <c r="A26" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>227</v>
+      </c>
       <c r="C26" s="59"/>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
       <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
+      <c r="G26" s="68" t="s">
+        <v>182</v>
+      </c>
       <c r="H26" s="68"/>
       <c r="I26" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J26" s="59"/>
+      <c r="J26" s="59" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="48" t="s">
@@ -5161,9 +5242,13 @@
       <c r="I27" s="49"/>
       <c r="J27" s="49"/>
     </row>
-    <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="72"/>
-      <c r="B28" s="73"/>
+    <row r="28" spans="1:10" ht="30">
+      <c r="A28" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="76" t="s">
+        <v>229</v>
+      </c>
       <c r="C28" s="74"/>
       <c r="D28" s="74"/>
       <c r="E28" s="72"/>
@@ -5173,11 +5258,17 @@
       <c r="I28" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J28" s="72"/>
-    </row>
-    <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="72"/>
-      <c r="B29" s="76"/>
+      <c r="J28" s="72" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30">
+      <c r="A29" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="76" t="s">
+        <v>230</v>
+      </c>
       <c r="C29" s="72"/>
       <c r="D29" s="72"/>
       <c r="E29" s="72"/>
@@ -5187,11 +5278,17 @@
       <c r="I29" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J29" s="72"/>
-    </row>
-    <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="72"/>
-      <c r="B30" s="73"/>
+      <c r="J29" s="72" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45">
+      <c r="A30" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="76" t="s">
+        <v>234</v>
+      </c>
       <c r="C30" s="72"/>
       <c r="D30" s="72"/>
       <c r="E30" s="72"/>
@@ -5201,11 +5298,17 @@
       <c r="I30" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J30" s="72"/>
-    </row>
-    <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
+      <c r="J30" s="72" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30">
+      <c r="A31" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="76" t="s">
+        <v>236</v>
+      </c>
       <c r="C31" s="72"/>
       <c r="D31" s="72"/>
       <c r="E31" s="72"/>
@@ -5215,77 +5318,81 @@
       <c r="I31" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J31" s="72"/>
-    </row>
-    <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="72"/>
-      <c r="B32" s="73"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="J32" s="72"/>
+      <c r="J31" s="72" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="72"/>
-      <c r="B33" s="73"/>
+      <c r="A33" s="72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="76"/>
       <c r="C33" s="72"/>
       <c r="D33" s="72"/>
       <c r="E33" s="72"/>
       <c r="F33" s="72"/>
       <c r="G33" s="72"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="68" t="s">
+      <c r="H33" s="77"/>
+      <c r="I33" s="71" t="s">
         <v>171</v>
       </c>
       <c r="J33" s="72"/>
     </row>
     <row r="34" spans="1:10" ht="15">
       <c r="A34" s="72"/>
-      <c r="B34" s="73"/>
+      <c r="B34" s="76"/>
       <c r="C34" s="72"/>
       <c r="D34" s="72"/>
       <c r="E34" s="72"/>
       <c r="F34" s="72"/>
       <c r="G34" s="72"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="68" t="s">
+      <c r="H34" s="77"/>
+      <c r="I34" s="71" t="s">
         <v>171</v>
       </c>
       <c r="J34" s="72"/>
     </row>
     <row r="35" spans="1:10" ht="15">
       <c r="A35" s="72"/>
-      <c r="B35" s="73"/>
+      <c r="B35" s="76"/>
       <c r="C35" s="72"/>
       <c r="D35" s="72"/>
       <c r="E35" s="72"/>
       <c r="F35" s="72"/>
       <c r="G35" s="72"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="68" t="s">
+      <c r="H35" s="77"/>
+      <c r="I35" s="71" t="s">
         <v>171</v>
       </c>
       <c r="J35" s="72"/>
     </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
+    <row r="36" spans="1:10" ht="15">
+      <c r="A36" s="72"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="71" t="s">
+        <v>171</v>
+      </c>
+      <c r="J36" s="72"/>
     </row>
     <row r="37" spans="1:10" ht="15">
       <c r="A37" s="72"/>
@@ -5385,72 +5492,16 @@
       </c>
       <c r="J43" s="72"/>
     </row>
-    <row r="44" spans="1:10" ht="15">
-      <c r="A44" s="72"/>
-      <c r="B44" s="76"/>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="77"/>
-      <c r="I44" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J44" s="72"/>
-    </row>
-    <row r="45" spans="1:10" ht="15">
-      <c r="A45" s="72"/>
-      <c r="B45" s="76"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
-      <c r="E45" s="72"/>
-      <c r="F45" s="72"/>
-      <c r="G45" s="72"/>
-      <c r="H45" s="77"/>
-      <c r="I45" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J45" s="72"/>
-    </row>
-    <row r="46" spans="1:10" ht="15">
-      <c r="A46" s="72"/>
-      <c r="B46" s="76"/>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="77"/>
-      <c r="I46" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J46" s="72"/>
-    </row>
-    <row r="47" spans="1:10" ht="15">
-      <c r="A47" s="72"/>
-      <c r="B47" s="76"/>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
-      <c r="E47" s="72"/>
-      <c r="F47" s="72"/>
-      <c r="G47" s="72"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J47" s="72"/>
-    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A23:J23"/>
     <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A32:J32"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A11:J11"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
@@ -5466,7 +5517,7 @@
       <formula>"VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37:I1048576 I28:I35 I4:I6 I13:I15 I10:I11 I23:I26 I17:I21">
+  <conditionalFormatting sqref="I33:I1048576 I18:I22 I24:I26 I4:I6 I10 I12:I16 I28:I31">
     <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NOT VERIFIED">
       <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I4)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added requirements for each subsystem
</commit_message>
<xml_diff>
--- a/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
+++ b/CMQA/Requirements Verification Matrix/RCL-RVM-CMQA1 Rascal Requirements Verification Matrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="240">
   <si>
     <t>Document Title</t>
   </si>
@@ -668,9 +668,6 @@
     <t>NOT VERIFIED</t>
   </si>
   <si>
-    <t>Mission Operations Requirements</t>
-  </si>
-  <si>
     <t>Power Requirements</t>
   </si>
   <si>
@@ -707,36 +704,21 @@
     <t>The spacecraft will utilize the CubeSat standard architecture</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>The mission will consist of two identical spacecraft</t>
   </si>
   <si>
-    <t>Risk Mitigation</t>
-  </si>
-  <si>
     <t>The two spacecraft must be able to integrate into the same dispenser</t>
   </si>
   <si>
-    <t>Launch Requirement</t>
-  </si>
-  <si>
     <t>The two spacecraft will be conjoined for integration into dispenser</t>
   </si>
   <si>
     <t>The two spacecraft will be capable of separating in orbit</t>
   </si>
   <si>
-    <t>Mission Requirements</t>
-  </si>
-  <si>
     <t>The spacecraft must be capable of determining relative distance between it and a resident space object</t>
   </si>
   <si>
-    <t>Mission Operations Requiremetns</t>
-  </si>
-  <si>
     <t>RCL-MOP1-1</t>
   </si>
   <si>
@@ -758,33 +740,15 @@
     <t>Mission Operations Sub-Requirements</t>
   </si>
   <si>
-    <t>Mission Operations Requirment</t>
-  </si>
-  <si>
     <t>The spacecraft will utilize a Power Subsystem</t>
   </si>
   <si>
-    <t>RCL-MOP1-2-CDH</t>
-  </si>
-  <si>
-    <t>RCL-MOP1-3-COM</t>
-  </si>
-  <si>
     <t>RCL-MOP2-PWR</t>
   </si>
   <si>
     <t>RCL-RFP-PRP</t>
   </si>
   <si>
-    <t>RCL-MOP1-1-ADC</t>
-  </si>
-  <si>
-    <t>Structure System</t>
-  </si>
-  <si>
-    <t>Structure Sub-Requirements</t>
-  </si>
-  <si>
     <t>RCL-STR</t>
   </si>
   <si>
@@ -803,6 +767,9 @@
     <t>RCL-STR-5</t>
   </si>
   <si>
+    <t>Propulsion Requirements</t>
+  </si>
+  <si>
     <t>RCL-RFP1</t>
   </si>
   <si>
@@ -821,12 +788,6 @@
     <t xml:space="preserve">The spacecraft will utilize a Propulsion Subsystem </t>
   </si>
   <si>
-    <t>RFP Requirements 1-3</t>
-  </si>
-  <si>
-    <t>Mission Operations Requirement 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">The spacecraft will utilize an Attitude Determination and Control Subsystem </t>
   </si>
   <si>
@@ -864,6 +825,51 @@
   </si>
   <si>
     <t>Attitude Determination and Control Requirements</t>
+  </si>
+  <si>
+    <t>Communications Requirements</t>
+  </si>
+  <si>
+    <t>The communicaton subsystem will utilize a radio for transmitting data to the ground</t>
+  </si>
+  <si>
+    <t>A link budget will be created that ensures that the power level, frequency, and altitudes over which the spacecraft transmits data are sufficient to produce a signal to noise ratio on the ground that is greater than one</t>
+  </si>
+  <si>
+    <t>Command and Data Handling Requirements</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-ADC</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-CDH</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-COM</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-COM1</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-COM2</t>
+  </si>
+  <si>
+    <t>The Command and Data Handling subsystem will be capable of managing the operation of each subystem of the spacecraft, as well as the communication of data between said subsystems</t>
+  </si>
+  <si>
+    <t>Structures Requirements</t>
+  </si>
+  <si>
+    <t>The ADC subsystem will be capable of autonomously commanding the propulsion system to perform the orbital maneuvers associated with the RFP requirements</t>
+  </si>
+  <si>
+    <t>RCL-MOP1-ADC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The propulsion subsystem will be capable of executing orbital maneuvers issued to it from the ADC subsystem </t>
+  </si>
+  <si>
+    <t>RCL-RFP-PRP1</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1439,6 +1445,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1464,12 +1476,129 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -4676,10 +4805,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4708,7 +4837,7 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H1" s="50" t="s">
         <v>53</v>
@@ -4717,7 +4846,7 @@
         <v>170</v>
       </c>
       <c r="J1" s="52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.25">
@@ -4755,91 +4884,91 @@
       <c r="J3" s="49"/>
     </row>
     <row r="4" spans="1:10" ht="45">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="J4" s="74" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45">
+      <c r="A5" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="78" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="J4" s="72" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45">
-      <c r="A5" s="72" t="s">
+      <c r="J5" s="74" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45">
+      <c r="A6" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77" t="s">
+      <c r="B6" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79" t="s">
         <v>171</v>
       </c>
-      <c r="J5" s="72" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="45">
-      <c r="A6" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="76" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72" t="s">
-        <v>181</v>
-      </c>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77" t="s">
-        <v>171</v>
-      </c>
-      <c r="J6" s="72" t="s">
-        <v>219</v>
+      <c r="J6" s="74" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45">
       <c r="A7" s="61" t="s">
         <v>167</v>
       </c>
-      <c r="B7" s="78" t="s">
-        <v>179</v>
+      <c r="B7" s="80" t="s">
+        <v>178</v>
       </c>
       <c r="C7" s="57"/>
       <c r="D7" s="57"/>
       <c r="E7" s="57"/>
       <c r="F7" s="57"/>
       <c r="G7" s="63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H7" s="63"/>
       <c r="I7" s="62" t="s">
         <v>171</v>
       </c>
       <c r="J7" s="64" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
@@ -4847,26 +4976,26 @@
         <v>167</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
       <c r="E8" s="57"/>
       <c r="F8" s="57"/>
       <c r="G8" s="63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H8" s="63"/>
       <c r="I8" s="62" t="s">
         <v>171</v>
       </c>
       <c r="J8" s="64" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="48" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B9" s="49"/>
       <c r="C9" s="49"/>
@@ -4879,629 +5008,574 @@
       <c r="J9" s="49"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="73" t="s">
-        <v>228</v>
-      </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="77" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="59" t="s">
+      <c r="B10" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J10" s="72" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="A12" s="72" t="s">
-        <v>177</v>
+      <c r="J10" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30">
+      <c r="A11" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J11" s="59" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30">
+      <c r="A12" s="61" t="s">
+        <v>14</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C12" s="59"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
       <c r="F12" s="59"/>
-      <c r="G12" s="59" t="s">
-        <v>185</v>
-      </c>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59" t="s">
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J12" s="56" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="72" t="s">
+      <c r="J12" s="59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A13" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59" t="s">
-        <v>187</v>
-      </c>
-      <c r="H13" s="59"/>
+      <c r="B13" s="75" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="81"/>
       <c r="I13" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="J13" s="56" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A14" s="72" t="s">
+      <c r="J13" s="74" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1">
+      <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
       <c r="E14" s="59"/>
       <c r="F14" s="59"/>
-      <c r="G14" s="59" t="s">
-        <v>189</v>
-      </c>
+      <c r="G14" s="68"/>
       <c r="H14" s="68"/>
       <c r="I14" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J14" s="56" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="72" t="s">
+      <c r="J14" s="59" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15">
+      <c r="A15" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="59"/>
       <c r="E15" s="59"/>
       <c r="F15" s="59"/>
-      <c r="G15" s="59" t="s">
-        <v>187</v>
-      </c>
+      <c r="G15" s="68"/>
       <c r="H15" s="68"/>
       <c r="I15" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J15" s="56" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="72" t="s">
+      <c r="J15" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+    </row>
+    <row r="17" spans="1:10" ht="30">
+      <c r="A17" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59" t="s">
-        <v>192</v>
-      </c>
-      <c r="H16" s="68"/>
-      <c r="I16" s="68" t="s">
+      <c r="B17" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J16" s="56" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="48" t="s">
-        <v>196</v>
-      </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="J17" s="59" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="65" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="C18" s="59"/>
       <c r="D18" s="59"/>
       <c r="E18" s="59"/>
       <c r="F18" s="59"/>
-      <c r="G18" s="68" t="s">
-        <v>194</v>
-      </c>
+      <c r="G18" s="68"/>
       <c r="H18" s="68"/>
       <c r="I18" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J18" s="59" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15">
       <c r="A19" s="61" t="s">
         <v>14</v>
       </c>
       <c r="B19" s="65" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="C19" s="59"/>
       <c r="D19" s="59"/>
       <c r="E19" s="59"/>
       <c r="F19" s="59"/>
-      <c r="G19" s="68" t="s">
-        <v>172</v>
-      </c>
+      <c r="G19" s="68"/>
       <c r="H19" s="68"/>
       <c r="I19" s="68" t="s">
         <v>171</v>
       </c>
       <c r="J19" s="59" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="65" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="68" t="s">
-        <v>172</v>
-      </c>
-      <c r="H20" s="68"/>
-      <c r="I20" s="68" t="s">
-        <v>171</v>
-      </c>
-      <c r="J20" s="59" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="30">
-      <c r="A21" s="61" t="s">
-        <v>14</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+    </row>
+    <row r="21" spans="1:10" ht="15">
+      <c r="A21" s="74" t="s">
+        <v>176</v>
       </c>
       <c r="B21" s="65" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="C21" s="59"/>
       <c r="D21" s="59"/>
       <c r="E21" s="59"/>
       <c r="F21" s="59"/>
-      <c r="G21" s="68" t="s">
-        <v>223</v>
-      </c>
-      <c r="H21" s="68"/>
-      <c r="I21" s="68" t="s">
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="J21" s="59" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30">
-      <c r="A22" s="61" t="s">
+      <c r="J21" s="56" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15">
+      <c r="A22" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="65" t="s">
-        <v>203</v>
+      <c r="B22" s="66" t="s">
+        <v>184</v>
       </c>
       <c r="C22" s="59"/>
       <c r="D22" s="59"/>
       <c r="E22" s="59"/>
       <c r="F22" s="59"/>
-      <c r="G22" s="68" t="s">
-        <v>224</v>
-      </c>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68" t="s">
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="J22" s="59" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="48" t="s">
+      <c r="J22" s="56" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-    </row>
-    <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="61" t="s">
+    </row>
+    <row r="23" spans="1:10" ht="30">
+      <c r="A23" s="74" t="s">
         <v>14</v>
       </c>
+      <c r="B23" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68" t="s">
+        <v>171</v>
+      </c>
+      <c r="J23" s="56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15">
+      <c r="A24" s="74" t="s">
+        <v>14</v>
+      </c>
       <c r="B24" s="65" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
       <c r="C24" s="59"/>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
-      <c r="G24" s="68" t="s">
-        <v>202</v>
-      </c>
+      <c r="G24" s="59"/>
       <c r="H24" s="68"/>
       <c r="I24" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J24" s="59" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="61" t="s">
+      <c r="J24" s="56" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15">
+      <c r="A25" s="74" t="s">
         <v>14</v>
       </c>
       <c r="B25" s="65" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
-      <c r="G25" s="68" t="s">
-        <v>182</v>
-      </c>
+      <c r="G25" s="59"/>
       <c r="H25" s="68"/>
       <c r="I25" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J25" s="59" t="s">
+      <c r="J25" s="56" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="61" t="s">
+    <row r="26" spans="1:10">
+      <c r="A26" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+    </row>
+    <row r="27" spans="1:10" ht="30">
+      <c r="A27" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="65" t="s">
-        <v>227</v>
-      </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="68" t="s">
-        <v>182</v>
-      </c>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68" t="s">
+      <c r="B27" s="78" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" s="76"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="76"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J26" s="59" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
+      <c r="J27" s="74" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="30">
-      <c r="A28" s="72" t="s">
+      <c r="A28" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="76" t="s">
-        <v>229</v>
+      <c r="B28" s="78" t="s">
+        <v>217</v>
       </c>
       <c r="C28" s="74"/>
       <c r="D28" s="74"/>
-      <c r="E28" s="72"/>
+      <c r="E28" s="74"/>
       <c r="F28" s="74"/>
       <c r="G28" s="74"/>
-      <c r="H28" s="75"/>
+      <c r="H28" s="77"/>
       <c r="I28" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J28" s="72" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="72" t="s">
+      <c r="J28" s="74" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45">
+      <c r="A29" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="76" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="75"/>
+      <c r="B29" s="78" t="s">
+        <v>221</v>
+      </c>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="77"/>
       <c r="I29" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J29" s="72" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="45">
-      <c r="A30" s="72" t="s">
+      <c r="J29" s="74" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30">
+      <c r="A30" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="76" t="s">
-        <v>234</v>
-      </c>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="75"/>
+      <c r="B30" s="78" t="s">
+        <v>223</v>
+      </c>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="77"/>
       <c r="I30" s="68" t="s">
         <v>171</v>
       </c>
-      <c r="J30" s="72" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="30">
-      <c r="A31" s="72" t="s">
+      <c r="J30" s="74" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="49"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+    </row>
+    <row r="32" spans="1:10" ht="45">
+      <c r="A32" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="76" t="s">
+      <c r="B32" s="84" t="s">
         <v>236</v>
       </c>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="68" t="s">
+      <c r="C32" s="83"/>
+      <c r="D32" s="83"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="J31" s="72" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="48" t="s">
+      <c r="J32" s="83" t="s">
         <v>237</v>
       </c>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-    </row>
-    <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="76"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="B33" s="72"/>
       <c r="C33" s="72"/>
       <c r="D33" s="72"/>
       <c r="E33" s="72"/>
       <c r="F33" s="72"/>
       <c r="G33" s="72"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="71" t="s">
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+    </row>
+    <row r="34" spans="1:10" ht="30">
+      <c r="A34" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="84" t="s">
+        <v>238</v>
+      </c>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="82" t="s">
         <v>171</v>
       </c>
-      <c r="J33" s="72"/>
-    </row>
-    <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="72"/>
-      <c r="B34" s="76"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="71" t="s">
+      <c r="J34" s="83" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="B35" s="49"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+    </row>
+    <row r="36" spans="1:10" ht="30">
+      <c r="A36" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="78" t="s">
+        <v>226</v>
+      </c>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="J34" s="72"/>
-    </row>
-    <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="72"/>
-      <c r="B35" s="76"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="71" t="s">
+      <c r="J36" s="59" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="60">
+      <c r="A37" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="78" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="J35" s="72"/>
-    </row>
-    <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="72"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="71" t="s">
+      <c r="J37" s="59" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="48" t="s">
+        <v>228</v>
+      </c>
+      <c r="B38" s="49"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+    </row>
+    <row r="39" spans="1:10" ht="45">
+      <c r="A39" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="78" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="J36" s="72"/>
-    </row>
-    <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="72"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J37" s="72"/>
-    </row>
-    <row r="38" spans="1:10" ht="15">
-      <c r="A38" s="72"/>
-      <c r="B38" s="76"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J38" s="72"/>
-    </row>
-    <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="72"/>
-      <c r="B39" s="76"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J39" s="72"/>
-    </row>
-    <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="72"/>
-      <c r="B40" s="76"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="72"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J40" s="72"/>
-    </row>
-    <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="72"/>
-      <c r="B41" s="76"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J41" s="72"/>
-    </row>
-    <row r="42" spans="1:10" ht="15">
-      <c r="A42" s="72"/>
-      <c r="B42" s="76"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="72"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J42" s="72"/>
-    </row>
-    <row r="43" spans="1:10" ht="15">
-      <c r="A43" s="72"/>
-      <c r="B43" s="76"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="71" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="72"/>
+      <c r="J39" s="74" t="s">
+        <v>230</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A32:J32"/>
+  <mergeCells count="15">
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A31:J31"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A20:J20"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
@@ -5510,21 +5584,43 @@
     <mergeCell ref="H1:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:I8">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NOT VERIFIED">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="NOT VERIFIED">
       <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I7)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I33:I1048576 I18:I22 I24:I26 I4:I6 I10 I12:I16 I28:I31">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NOT VERIFIED">
+  <conditionalFormatting sqref="I36:I37 I39:I1048576 I21:I25 I27:I30 I10:I15 I17:I19 I4:I6">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="NOT VERIFIED">
       <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="VERIFIED">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="VERIFIED">
       <formula>NOT(ISERROR(SEARCH("VERIFIED",I4)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"NOT VERIFIED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I32">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",I32)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+      <formula>"NOT VERIFIED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NOT VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("NOT VERIFIED",I34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="VERIFIED">
+      <formula>NOT(ISERROR(SEARCH("VERIFIED",I34)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NOT VERIFIED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>